<commit_message>
changed date format in template charts
</commit_message>
<xml_diff>
--- a/code/scripts/RACF_Fuel_factsheet_template.xlsx
+++ b/code/scripts/RACF_Fuel_factsheet_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="master" sheetId="1" state="visible" r:id="rId2"/>
@@ -604,11 +604,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="MM/DD/YYYY\ HH:MM:SS"/>
     <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
-    <numFmt numFmtId="167" formatCode="DD\-MM\-YYYY"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -728,8 +727,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="22" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -864,11 +863,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="37431270"/>
-        <c:axId val="86811736"/>
+        <c:axId val="34724557"/>
+        <c:axId val="25069989"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="37431270"/>
+        <c:axId val="34724557"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -896,14 +895,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86811736"/>
+        <c:crossAx val="25069989"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="86811736"/>
+        <c:axId val="25069989"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -940,7 +939,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="37431270"/>
+        <c:crossAx val="34724557"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4227,17 +4226,17 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="6354305"/>
-        <c:axId val="4402620"/>
+        <c:axId val="2381999"/>
+        <c:axId val="21891262"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="6354305"/>
+        <c:axId val="2381999"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="DD\-MM\-YYYY" sourceLinked="1"/>
+        <c:numFmt formatCode="DD/MM/YYYY" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4259,14 +4258,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4402620"/>
+        <c:crossAx val="21891262"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="4402620"/>
+        <c:axId val="21891262"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4301,7 +4300,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="6354305"/>
+        <c:crossAx val="2381999"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4358,10 +4357,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0755896226415094"/>
-          <c:y val="0.072019923268493"/>
-          <c:w val="0.898270440251572"/>
-          <c:h val="0.759036144578313"/>
+          <c:x val="0.0755925940485082"/>
+          <c:y val="0.0720247711362413"/>
+          <c:w val="0.898227131569637"/>
+          <c:h val="0.758952611739365"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -7597,17 +7596,17 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="35644525"/>
-        <c:axId val="2533900"/>
+        <c:axId val="58992009"/>
+        <c:axId val="57152822"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="35644525"/>
+        <c:axId val="58992009"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="DD\-MM\-YYYY" sourceLinked="1"/>
+        <c:numFmt formatCode="DD/MM/YYYY" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -7629,14 +7628,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2533900"/>
+        <c:crossAx val="57152822"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2533900"/>
+        <c:axId val="57152822"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7671,7 +7670,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="35644525"/>
+        <c:crossAx val="58992009"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7722,7 +7721,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>40320</xdr:colOff>
+      <xdr:colOff>40680</xdr:colOff>
       <xdr:row>259</xdr:row>
       <xdr:rowOff>57960</xdr:rowOff>
     </xdr:from>
@@ -7730,7 +7729,7 @@
       <xdr:col>17</xdr:col>
       <xdr:colOff>483840</xdr:colOff>
       <xdr:row>277</xdr:row>
-      <xdr:rowOff>138600</xdr:rowOff>
+      <xdr:rowOff>138240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7738,8 +7737,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10731600" y="48998520"/>
-        <a:ext cx="5755320" cy="3235320"/>
+        <a:off x="10731960" y="49012560"/>
+        <a:ext cx="5754960" cy="3234960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7763,9 +7762,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>216360</xdr:colOff>
+      <xdr:colOff>216000</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>7920</xdr:rowOff>
+      <xdr:rowOff>7560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7774,7 +7773,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="29520" y="28800"/>
-        <a:ext cx="8314560" cy="4855680"/>
+        <a:ext cx="8314200" cy="4855320"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7798,9 +7797,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>217800</xdr:colOff>
+      <xdr:colOff>217440</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>146880</xdr:rowOff>
+      <xdr:rowOff>146520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7809,7 +7808,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="360" y="360"/>
-        <a:ext cx="9158040" cy="5348160"/>
+        <a:ext cx="9157680" cy="5347800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7830,7 +7829,7 @@
   <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A:A"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8399,7 +8398,7 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A:A"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9013,7 +9012,7 @@
   <dimension ref="A1:C255"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A:A"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9024,7 +9023,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>185</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -9035,7 +9034,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="n">
+      <c r="A2" s="4" t="n">
         <v>43859.0416666667</v>
       </c>
       <c r="B2" s="2" t="n">
@@ -9046,7 +9045,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="n">
+      <c r="A3" s="4" t="n">
         <v>43858.0416666667</v>
       </c>
       <c r="B3" s="2" t="n">
@@ -9057,7 +9056,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="n">
+      <c r="A4" s="4" t="n">
         <v>43857.0416666667</v>
       </c>
       <c r="B4" s="2" t="n">
@@ -9068,7 +9067,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="n">
+      <c r="A5" s="4" t="n">
         <v>43854.0416666667</v>
       </c>
       <c r="B5" s="2" t="n">
@@ -9079,7 +9078,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="n">
+      <c r="A6" s="4" t="n">
         <v>43853.0416666667</v>
       </c>
       <c r="B6" s="2" t="n">
@@ -9090,7 +9089,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="n">
+      <c r="A7" s="4" t="n">
         <v>43852.0416666667</v>
       </c>
       <c r="B7" s="2" t="n">
@@ -9101,7 +9100,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="n">
+      <c r="A8" s="4" t="n">
         <v>43851.0416666667</v>
       </c>
       <c r="B8" s="2" t="n">
@@ -9112,7 +9111,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="n">
+      <c r="A9" s="4" t="n">
         <v>43850.0416666667</v>
       </c>
       <c r="B9" s="2" t="n">
@@ -9123,7 +9122,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="n">
+      <c r="A10" s="4" t="n">
         <v>43847.0416666667</v>
       </c>
       <c r="B10" s="2" t="n">
@@ -9134,7 +9133,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="n">
+      <c r="A11" s="4" t="n">
         <v>43846.0416666667</v>
       </c>
       <c r="B11" s="2" t="n">
@@ -9145,7 +9144,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="n">
+      <c r="A12" s="4" t="n">
         <v>43845.0416666667</v>
       </c>
       <c r="B12" s="2" t="n">
@@ -9156,7 +9155,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="n">
+      <c r="A13" s="4" t="n">
         <v>43844.0416666667</v>
       </c>
       <c r="B13" s="2" t="n">
@@ -9167,7 +9166,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="n">
+      <c r="A14" s="4" t="n">
         <v>43843.0416666667</v>
       </c>
       <c r="B14" s="2" t="n">
@@ -9178,7 +9177,7 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="n">
+      <c r="A15" s="4" t="n">
         <v>43840.0416666667</v>
       </c>
       <c r="B15" s="2" t="n">
@@ -9189,7 +9188,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5" t="n">
+      <c r="A16" s="4" t="n">
         <v>43839.0416666667</v>
       </c>
       <c r="B16" s="2" t="n">
@@ -9200,7 +9199,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5" t="n">
+      <c r="A17" s="4" t="n">
         <v>43838.0416666667</v>
       </c>
       <c r="B17" s="2" t="n">
@@ -9211,7 +9210,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5" t="n">
+      <c r="A18" s="4" t="n">
         <v>43837.0416666667</v>
       </c>
       <c r="B18" s="2" t="n">
@@ -9222,7 +9221,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5" t="n">
+      <c r="A19" s="4" t="n">
         <v>43836.0416666667</v>
       </c>
       <c r="B19" s="2" t="n">
@@ -9233,7 +9232,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5" t="n">
+      <c r="A20" s="4" t="n">
         <v>43833.0416666667</v>
       </c>
       <c r="B20" s="2" t="n">
@@ -9244,7 +9243,7 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="5" t="n">
+      <c r="A21" s="4" t="n">
         <v>43832.0416666667</v>
       </c>
       <c r="B21" s="2" t="n">
@@ -9255,7 +9254,7 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="5" t="n">
+      <c r="A22" s="4" t="n">
         <v>43830.0416666667</v>
       </c>
       <c r="B22" s="2" t="n">
@@ -9266,7 +9265,7 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="5" t="n">
+      <c r="A23" s="4" t="n">
         <v>43829.0416666667</v>
       </c>
       <c r="B23" s="2" t="n">
@@ -9277,7 +9276,7 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="5" t="n">
+      <c r="A24" s="4" t="n">
         <v>43826.0416666667</v>
       </c>
       <c r="B24" s="2" t="n">
@@ -9288,7 +9287,7 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="5" t="n">
+      <c r="A25" s="4" t="n">
         <v>43823.0416666667</v>
       </c>
       <c r="B25" s="2" t="n">
@@ -9299,7 +9298,7 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="5" t="n">
+      <c r="A26" s="4" t="n">
         <v>43822.0416666667</v>
       </c>
       <c r="B26" s="2" t="n">
@@ -9310,7 +9309,7 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="5" t="n">
+      <c r="A27" s="4" t="n">
         <v>43819.0416666667</v>
       </c>
       <c r="B27" s="2" t="n">
@@ -9321,7 +9320,7 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="5" t="n">
+      <c r="A28" s="4" t="n">
         <v>43818.0416666667</v>
       </c>
       <c r="B28" s="2" t="n">
@@ -9332,7 +9331,7 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="5" t="n">
+      <c r="A29" s="4" t="n">
         <v>43817.0416666667</v>
       </c>
       <c r="B29" s="2" t="n">
@@ -9343,7 +9342,7 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="5" t="n">
+      <c r="A30" s="4" t="n">
         <v>43816.0416666667</v>
       </c>
       <c r="B30" s="2" t="n">
@@ -9354,7 +9353,7 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="5" t="n">
+      <c r="A31" s="4" t="n">
         <v>43815.0416666667</v>
       </c>
       <c r="B31" s="2" t="n">
@@ -9365,7 +9364,7 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="5" t="n">
+      <c r="A32" s="4" t="n">
         <v>43812.0416666667</v>
       </c>
       <c r="B32" s="2" t="n">
@@ -9376,7 +9375,7 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="5" t="n">
+      <c r="A33" s="4" t="n">
         <v>43811.0416666667</v>
       </c>
       <c r="B33" s="2" t="n">
@@ -9387,7 +9386,7 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="5" t="n">
+      <c r="A34" s="4" t="n">
         <v>43810.0416666667</v>
       </c>
       <c r="B34" s="2" t="n">
@@ -9398,7 +9397,7 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="5" t="n">
+      <c r="A35" s="4" t="n">
         <v>43809.0416666667</v>
       </c>
       <c r="B35" s="2" t="n">
@@ -9409,7 +9408,7 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="5" t="n">
+      <c r="A36" s="4" t="n">
         <v>43808.0416666667</v>
       </c>
       <c r="B36" s="2" t="n">
@@ -9420,7 +9419,7 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="5" t="n">
+      <c r="A37" s="4" t="n">
         <v>43805.0416666667</v>
       </c>
       <c r="B37" s="2" t="n">
@@ -9431,7 +9430,7 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="5" t="n">
+      <c r="A38" s="4" t="n">
         <v>43804.0416666667</v>
       </c>
       <c r="B38" s="2" t="n">
@@ -9442,7 +9441,7 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="5" t="n">
+      <c r="A39" s="4" t="n">
         <v>43803.0416666667</v>
       </c>
       <c r="B39" s="2" t="n">
@@ -9453,7 +9452,7 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="5" t="n">
+      <c r="A40" s="4" t="n">
         <v>43802.0416666667</v>
       </c>
       <c r="B40" s="2" t="n">
@@ -9464,7 +9463,7 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="5" t="n">
+      <c r="A41" s="4" t="n">
         <v>43801.0416666667</v>
       </c>
       <c r="B41" s="2" t="n">
@@ -9475,7 +9474,7 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="5" t="n">
+      <c r="A42" s="4" t="n">
         <v>43798.0416666667</v>
       </c>
       <c r="B42" s="2" t="n">
@@ -9486,7 +9485,7 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="5" t="n">
+      <c r="A43" s="4" t="n">
         <v>43797.0416666667</v>
       </c>
       <c r="B43" s="2" t="n">
@@ -9497,7 +9496,7 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="5" t="n">
+      <c r="A44" s="4" t="n">
         <v>43796.0416666667</v>
       </c>
       <c r="B44" s="2" t="n">
@@ -9508,7 +9507,7 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="5" t="n">
+      <c r="A45" s="4" t="n">
         <v>43795.0416666667</v>
       </c>
       <c r="B45" s="2" t="n">
@@ -9519,7 +9518,7 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="5" t="n">
+      <c r="A46" s="4" t="n">
         <v>43794.0416666667</v>
       </c>
       <c r="B46" s="2" t="n">
@@ -9530,7 +9529,7 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="5" t="n">
+      <c r="A47" s="4" t="n">
         <v>43791.0416666667</v>
       </c>
       <c r="B47" s="2" t="n">
@@ -9541,7 +9540,7 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="5" t="n">
+      <c r="A48" s="4" t="n">
         <v>43790.0416666667</v>
       </c>
       <c r="B48" s="2" t="n">
@@ -9552,7 +9551,7 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="5" t="n">
+      <c r="A49" s="4" t="n">
         <v>43789.0416666667</v>
       </c>
       <c r="B49" s="2" t="n">
@@ -9563,7 +9562,7 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="5" t="n">
+      <c r="A50" s="4" t="n">
         <v>43788.0416666667</v>
       </c>
       <c r="B50" s="2" t="n">
@@ -9574,7 +9573,7 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="5" t="n">
+      <c r="A51" s="4" t="n">
         <v>43787.0416666667</v>
       </c>
       <c r="B51" s="2" t="n">
@@ -9585,7 +9584,7 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="5" t="n">
+      <c r="A52" s="4" t="n">
         <v>43784.0416666667</v>
       </c>
       <c r="B52" s="2" t="n">
@@ -9596,7 +9595,7 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="5" t="n">
+      <c r="A53" s="4" t="n">
         <v>43783.0416666667</v>
       </c>
       <c r="B53" s="2" t="n">
@@ -9607,7 +9606,7 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="5" t="n">
+      <c r="A54" s="4" t="n">
         <v>43782.0416666667</v>
       </c>
       <c r="B54" s="2" t="n">
@@ -9618,7 +9617,7 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="5" t="n">
+      <c r="A55" s="4" t="n">
         <v>43781.0416666667</v>
       </c>
       <c r="B55" s="2" t="n">
@@ -9629,7 +9628,7 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="5" t="n">
+      <c r="A56" s="4" t="n">
         <v>43780.0416666667</v>
       </c>
       <c r="B56" s="2" t="n">
@@ -9640,7 +9639,7 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="5" t="n">
+      <c r="A57" s="4" t="n">
         <v>43777.0416666667</v>
       </c>
       <c r="B57" s="2" t="n">
@@ -9651,7 +9650,7 @@
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="5" t="n">
+      <c r="A58" s="4" t="n">
         <v>43776.0416666667</v>
       </c>
       <c r="B58" s="2" t="n">
@@ -9662,7 +9661,7 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="5" t="n">
+      <c r="A59" s="4" t="n">
         <v>43775.0416666667</v>
       </c>
       <c r="B59" s="2" t="n">
@@ -9673,7 +9672,7 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="5" t="n">
+      <c r="A60" s="4" t="n">
         <v>43774.0416666667</v>
       </c>
       <c r="B60" s="2" t="n">
@@ -9684,7 +9683,7 @@
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="5" t="n">
+      <c r="A61" s="4" t="n">
         <v>43773.0416666667</v>
       </c>
       <c r="B61" s="2" t="n">
@@ -9695,7 +9694,7 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="5" t="n">
+      <c r="A62" s="4" t="n">
         <v>43770.0416666667</v>
       </c>
       <c r="B62" s="2" t="n">
@@ -9706,7 +9705,7 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="5" t="n">
+      <c r="A63" s="4" t="n">
         <v>43769.0416666667</v>
       </c>
       <c r="B63" s="2" t="n">
@@ -9717,7 +9716,7 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="5" t="n">
+      <c r="A64" s="4" t="n">
         <v>43768.0416666667</v>
       </c>
       <c r="B64" s="2" t="n">
@@ -9728,7 +9727,7 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="5" t="n">
+      <c r="A65" s="4" t="n">
         <v>43767.0416666667</v>
       </c>
       <c r="B65" s="2" t="n">
@@ -9739,7 +9738,7 @@
       </c>
     </row>
     <row r="66" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="5" t="n">
+      <c r="A66" s="4" t="n">
         <v>43766.0416666667</v>
       </c>
       <c r="B66" s="2" t="n">
@@ -9750,7 +9749,7 @@
       </c>
     </row>
     <row r="67" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="5" t="n">
+      <c r="A67" s="4" t="n">
         <v>43763.0833333333</v>
       </c>
       <c r="B67" s="2" t="n">
@@ -9761,7 +9760,7 @@
       </c>
     </row>
     <row r="68" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="5" t="n">
+      <c r="A68" s="4" t="n">
         <v>43762.0833333333</v>
       </c>
       <c r="B68" s="2" t="n">
@@ -9772,7 +9771,7 @@
       </c>
     </row>
     <row r="69" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="5" t="n">
+      <c r="A69" s="4" t="n">
         <v>43761.0833333333</v>
       </c>
       <c r="B69" s="2" t="n">
@@ -9783,7 +9782,7 @@
       </c>
     </row>
     <row r="70" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="5" t="n">
+      <c r="A70" s="4" t="n">
         <v>43760.0833333333</v>
       </c>
       <c r="B70" s="2" t="n">
@@ -9794,7 +9793,7 @@
       </c>
     </row>
     <row r="71" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="5" t="n">
+      <c r="A71" s="4" t="n">
         <v>43759.0833333333</v>
       </c>
       <c r="B71" s="2" t="n">
@@ -9805,7 +9804,7 @@
       </c>
     </row>
     <row r="72" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="5" t="n">
+      <c r="A72" s="4" t="n">
         <v>43756.0833333333</v>
       </c>
       <c r="B72" s="2" t="n">
@@ -9816,7 +9815,7 @@
       </c>
     </row>
     <row r="73" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="5" t="n">
+      <c r="A73" s="4" t="n">
         <v>43755.0833333333</v>
       </c>
       <c r="B73" s="2" t="n">
@@ -9827,7 +9826,7 @@
       </c>
     </row>
     <row r="74" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="5" t="n">
+      <c r="A74" s="4" t="n">
         <v>43754.0833333333</v>
       </c>
       <c r="B74" s="2" t="n">
@@ -9838,7 +9837,7 @@
       </c>
     </row>
     <row r="75" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="5" t="n">
+      <c r="A75" s="4" t="n">
         <v>43753.0833333333</v>
       </c>
       <c r="B75" s="2" t="n">
@@ -9849,7 +9848,7 @@
       </c>
     </row>
     <row r="76" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="5" t="n">
+      <c r="A76" s="4" t="n">
         <v>43752.0833333333</v>
       </c>
       <c r="B76" s="2" t="n">
@@ -9860,7 +9859,7 @@
       </c>
     </row>
     <row r="77" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="5" t="n">
+      <c r="A77" s="4" t="n">
         <v>43749.0833333333</v>
       </c>
       <c r="B77" s="2" t="n">
@@ -9871,7 +9870,7 @@
       </c>
     </row>
     <row r="78" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="5" t="n">
+      <c r="A78" s="4" t="n">
         <v>43748.0833333333</v>
       </c>
       <c r="B78" s="2" t="n">
@@ -9882,7 +9881,7 @@
       </c>
     </row>
     <row r="79" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="5" t="n">
+      <c r="A79" s="4" t="n">
         <v>43747.0833333333</v>
       </c>
       <c r="B79" s="2" t="n">
@@ -9893,7 +9892,7 @@
       </c>
     </row>
     <row r="80" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="5" t="n">
+      <c r="A80" s="4" t="n">
         <v>43746.0833333333</v>
       </c>
       <c r="B80" s="2" t="n">
@@ -9904,7 +9903,7 @@
       </c>
     </row>
     <row r="81" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="5" t="n">
+      <c r="A81" s="4" t="n">
         <v>43745.0833333333</v>
       </c>
       <c r="B81" s="2" t="n">
@@ -9915,7 +9914,7 @@
       </c>
     </row>
     <row r="82" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="5" t="n">
+      <c r="A82" s="4" t="n">
         <v>43742.0833333333</v>
       </c>
       <c r="B82" s="2" t="n">
@@ -9926,7 +9925,7 @@
       </c>
     </row>
     <row r="83" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="5" t="n">
+      <c r="A83" s="4" t="n">
         <v>43741.0833333333</v>
       </c>
       <c r="B83" s="2" t="n">
@@ -9937,7 +9936,7 @@
       </c>
     </row>
     <row r="84" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="5" t="n">
+      <c r="A84" s="4" t="n">
         <v>43740.0833333333</v>
       </c>
       <c r="B84" s="2" t="n">
@@ -9948,7 +9947,7 @@
       </c>
     </row>
     <row r="85" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="5" t="n">
+      <c r="A85" s="4" t="n">
         <v>43739.0833333333</v>
       </c>
       <c r="B85" s="2" t="n">
@@ -9959,7 +9958,7 @@
       </c>
     </row>
     <row r="86" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="5" t="n">
+      <c r="A86" s="4" t="n">
         <v>43738.0833333333</v>
       </c>
       <c r="B86" s="2" t="n">
@@ -9970,7 +9969,7 @@
       </c>
     </row>
     <row r="87" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="5" t="n">
+      <c r="A87" s="4" t="n">
         <v>43735.0833333333</v>
       </c>
       <c r="B87" s="2" t="n">
@@ -9981,7 +9980,7 @@
       </c>
     </row>
     <row r="88" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="5" t="n">
+      <c r="A88" s="4" t="n">
         <v>43734.0833333333</v>
       </c>
       <c r="B88" s="2" t="n">
@@ -9992,7 +9991,7 @@
       </c>
     </row>
     <row r="89" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="5" t="n">
+      <c r="A89" s="4" t="n">
         <v>43733.0833333333</v>
       </c>
       <c r="B89" s="2" t="n">
@@ -10003,7 +10002,7 @@
       </c>
     </row>
     <row r="90" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="5" t="n">
+      <c r="A90" s="4" t="n">
         <v>43732.0833333333</v>
       </c>
       <c r="B90" s="2" t="n">
@@ -10014,7 +10013,7 @@
       </c>
     </row>
     <row r="91" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="5" t="n">
+      <c r="A91" s="4" t="n">
         <v>43731.0833333333</v>
       </c>
       <c r="B91" s="2" t="n">
@@ -10025,7 +10024,7 @@
       </c>
     </row>
     <row r="92" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="5" t="n">
+      <c r="A92" s="4" t="n">
         <v>43728.0833333333</v>
       </c>
       <c r="B92" s="2" t="n">
@@ -10036,7 +10035,7 @@
       </c>
     </row>
     <row r="93" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="5" t="n">
+      <c r="A93" s="4" t="n">
         <v>43727.0833333333</v>
       </c>
       <c r="B93" s="2" t="n">
@@ -10047,7 +10046,7 @@
       </c>
     </row>
     <row r="94" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="5" t="n">
+      <c r="A94" s="4" t="n">
         <v>43726.0833333333</v>
       </c>
       <c r="B94" s="2" t="n">
@@ -10058,7 +10057,7 @@
       </c>
     </row>
     <row r="95" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="5" t="n">
+      <c r="A95" s="4" t="n">
         <v>43725.0833333333</v>
       </c>
       <c r="B95" s="2" t="n">
@@ -10069,7 +10068,7 @@
       </c>
     </row>
     <row r="96" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="5" t="n">
+      <c r="A96" s="4" t="n">
         <v>43724.0833333333</v>
       </c>
       <c r="B96" s="2" t="n">
@@ -10080,7 +10079,7 @@
       </c>
     </row>
     <row r="97" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="5" t="n">
+      <c r="A97" s="4" t="n">
         <v>43721.0833333333</v>
       </c>
       <c r="B97" s="2" t="n">
@@ -10091,7 +10090,7 @@
       </c>
     </row>
     <row r="98" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="5" t="n">
+      <c r="A98" s="4" t="n">
         <v>43720.0833333333</v>
       </c>
       <c r="B98" s="2" t="n">
@@ -10102,7 +10101,7 @@
       </c>
     </row>
     <row r="99" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="5" t="n">
+      <c r="A99" s="4" t="n">
         <v>43719.0833333333</v>
       </c>
       <c r="B99" s="2" t="n">
@@ -10113,7 +10112,7 @@
       </c>
     </row>
     <row r="100" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="5" t="n">
+      <c r="A100" s="4" t="n">
         <v>43718.0833333333</v>
       </c>
       <c r="B100" s="2" t="n">
@@ -10124,7 +10123,7 @@
       </c>
     </row>
     <row r="101" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="5" t="n">
+      <c r="A101" s="4" t="n">
         <v>43717.0833333333</v>
       </c>
       <c r="B101" s="2" t="n">
@@ -10135,7 +10134,7 @@
       </c>
     </row>
     <row r="102" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="5" t="n">
+      <c r="A102" s="4" t="n">
         <v>43714.0833333333</v>
       </c>
       <c r="B102" s="2" t="n">
@@ -10146,7 +10145,7 @@
       </c>
     </row>
     <row r="103" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="5" t="n">
+      <c r="A103" s="4" t="n">
         <v>43713.0833333333</v>
       </c>
       <c r="B103" s="2" t="n">
@@ -10157,7 +10156,7 @@
       </c>
     </row>
     <row r="104" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="5" t="n">
+      <c r="A104" s="4" t="n">
         <v>43712.0833333333</v>
       </c>
       <c r="B104" s="2" t="n">
@@ -10168,7 +10167,7 @@
       </c>
     </row>
     <row r="105" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="5" t="n">
+      <c r="A105" s="4" t="n">
         <v>43711.0833333333</v>
       </c>
       <c r="B105" s="2" t="n">
@@ -10179,7 +10178,7 @@
       </c>
     </row>
     <row r="106" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="5" t="n">
+      <c r="A106" s="4" t="n">
         <v>43710.0833333333</v>
       </c>
       <c r="B106" s="2" t="n">
@@ -10190,7 +10189,7 @@
       </c>
     </row>
     <row r="107" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="5" t="n">
+      <c r="A107" s="4" t="n">
         <v>43707.0833333333</v>
       </c>
       <c r="B107" s="2" t="n">
@@ -10201,7 +10200,7 @@
       </c>
     </row>
     <row r="108" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="5" t="n">
+      <c r="A108" s="4" t="n">
         <v>43706.0833333333</v>
       </c>
       <c r="B108" s="2" t="n">
@@ -10212,7 +10211,7 @@
       </c>
     </row>
     <row r="109" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="5" t="n">
+      <c r="A109" s="4" t="n">
         <v>43705.0833333333</v>
       </c>
       <c r="B109" s="2" t="n">
@@ -10223,7 +10222,7 @@
       </c>
     </row>
     <row r="110" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="5" t="n">
+      <c r="A110" s="4" t="n">
         <v>43704.0833333333</v>
       </c>
       <c r="B110" s="2" t="n">
@@ -10234,7 +10233,7 @@
       </c>
     </row>
     <row r="111" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="5" t="n">
+      <c r="A111" s="4" t="n">
         <v>43700.0833333333</v>
       </c>
       <c r="B111" s="2" t="n">
@@ -10245,7 +10244,7 @@
       </c>
     </row>
     <row r="112" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="5" t="n">
+      <c r="A112" s="4" t="n">
         <v>43699.0833333333</v>
       </c>
       <c r="B112" s="2" t="n">
@@ -10256,7 +10255,7 @@
       </c>
     </row>
     <row r="113" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="5" t="n">
+      <c r="A113" s="4" t="n">
         <v>43698.0833333333</v>
       </c>
       <c r="B113" s="2" t="n">
@@ -10267,7 +10266,7 @@
       </c>
     </row>
     <row r="114" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="5" t="n">
+      <c r="A114" s="4" t="n">
         <v>43697.0833333333</v>
       </c>
       <c r="B114" s="2" t="n">
@@ -10278,7 +10277,7 @@
       </c>
     </row>
     <row r="115" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="5" t="n">
+      <c r="A115" s="4" t="n">
         <v>43696.0833333333</v>
       </c>
       <c r="B115" s="2" t="n">
@@ -10289,7 +10288,7 @@
       </c>
     </row>
     <row r="116" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="5" t="n">
+      <c r="A116" s="4" t="n">
         <v>43693.0833333333</v>
       </c>
       <c r="B116" s="2" t="n">
@@ -10300,7 +10299,7 @@
       </c>
     </row>
     <row r="117" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="5" t="n">
+      <c r="A117" s="4" t="n">
         <v>43692.0833333333</v>
       </c>
       <c r="B117" s="2" t="n">
@@ -10311,7 +10310,7 @@
       </c>
     </row>
     <row r="118" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="5" t="n">
+      <c r="A118" s="4" t="n">
         <v>43691.0833333333</v>
       </c>
       <c r="B118" s="2" t="n">
@@ -10322,7 +10321,7 @@
       </c>
     </row>
     <row r="119" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="5" t="n">
+      <c r="A119" s="4" t="n">
         <v>43690.0833333333</v>
       </c>
       <c r="B119" s="2" t="n">
@@ -10333,7 +10332,7 @@
       </c>
     </row>
     <row r="120" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="5" t="n">
+      <c r="A120" s="4" t="n">
         <v>43689.0833333333</v>
       </c>
       <c r="B120" s="2" t="n">
@@ -10344,7 +10343,7 @@
       </c>
     </row>
     <row r="121" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="5" t="n">
+      <c r="A121" s="4" t="n">
         <v>43686.0833333333</v>
       </c>
       <c r="B121" s="2" t="n">
@@ -10355,7 +10354,7 @@
       </c>
     </row>
     <row r="122" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="5" t="n">
+      <c r="A122" s="4" t="n">
         <v>43685.0833333333</v>
       </c>
       <c r="B122" s="2" t="n">
@@ -10366,7 +10365,7 @@
       </c>
     </row>
     <row r="123" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="5" t="n">
+      <c r="A123" s="4" t="n">
         <v>43684.0833333333</v>
       </c>
       <c r="B123" s="2" t="n">
@@ -10377,7 +10376,7 @@
       </c>
     </row>
     <row r="124" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="5" t="n">
+      <c r="A124" s="4" t="n">
         <v>43683.0833333333</v>
       </c>
       <c r="B124" s="2" t="n">
@@ -10388,7 +10387,7 @@
       </c>
     </row>
     <row r="125" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="5" t="n">
+      <c r="A125" s="4" t="n">
         <v>43682.0833333333</v>
       </c>
       <c r="B125" s="2" t="n">
@@ -10399,7 +10398,7 @@
       </c>
     </row>
     <row r="126" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="5" t="n">
+      <c r="A126" s="4" t="n">
         <v>43679.0833333333</v>
       </c>
       <c r="B126" s="2" t="n">
@@ -10410,7 +10409,7 @@
       </c>
     </row>
     <row r="127" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="5" t="n">
+      <c r="A127" s="4" t="n">
         <v>43678.0833333333</v>
       </c>
       <c r="B127" s="2" t="n">
@@ -10421,7 +10420,7 @@
       </c>
     </row>
     <row r="128" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="5" t="n">
+      <c r="A128" s="4" t="n">
         <v>43677.0833333333</v>
       </c>
       <c r="B128" s="2" t="n">
@@ -10432,7 +10431,7 @@
       </c>
     </row>
     <row r="129" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="5" t="n">
+      <c r="A129" s="4" t="n">
         <v>43676.0833333333</v>
       </c>
       <c r="B129" s="2" t="n">
@@ -10443,7 +10442,7 @@
       </c>
     </row>
     <row r="130" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="5" t="n">
+      <c r="A130" s="4" t="n">
         <v>43675.0833333333</v>
       </c>
       <c r="B130" s="2" t="n">
@@ -10454,7 +10453,7 @@
       </c>
     </row>
     <row r="131" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="5" t="n">
+      <c r="A131" s="4" t="n">
         <v>43672.0833333333</v>
       </c>
       <c r="B131" s="2" t="n">
@@ -10465,7 +10464,7 @@
       </c>
     </row>
     <row r="132" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="5" t="n">
+      <c r="A132" s="4" t="n">
         <v>43671.0833333333</v>
       </c>
       <c r="B132" s="2" t="n">
@@ -10476,7 +10475,7 @@
       </c>
     </row>
     <row r="133" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="5" t="n">
+      <c r="A133" s="4" t="n">
         <v>43670.0833333333</v>
       </c>
       <c r="B133" s="2" t="n">
@@ -10487,7 +10486,7 @@
       </c>
     </row>
     <row r="134" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="5" t="n">
+      <c r="A134" s="4" t="n">
         <v>43669.0833333333</v>
       </c>
       <c r="B134" s="2" t="n">
@@ -10498,7 +10497,7 @@
       </c>
     </row>
     <row r="135" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="5" t="n">
+      <c r="A135" s="4" t="n">
         <v>43668.0833333333</v>
       </c>
       <c r="B135" s="2" t="n">
@@ -10509,7 +10508,7 @@
       </c>
     </row>
     <row r="136" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="5" t="n">
+      <c r="A136" s="4" t="n">
         <v>43665.0833333333</v>
       </c>
       <c r="B136" s="2" t="n">
@@ -10520,7 +10519,7 @@
       </c>
     </row>
     <row r="137" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="5" t="n">
+      <c r="A137" s="4" t="n">
         <v>43664.0833333333</v>
       </c>
       <c r="B137" s="2" t="n">
@@ -10531,7 +10530,7 @@
       </c>
     </row>
     <row r="138" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="5" t="n">
+      <c r="A138" s="4" t="n">
         <v>43663.0833333333</v>
       </c>
       <c r="B138" s="2" t="n">
@@ -10542,7 +10541,7 @@
       </c>
     </row>
     <row r="139" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="5" t="n">
+      <c r="A139" s="4" t="n">
         <v>43662.0833333333</v>
       </c>
       <c r="B139" s="2" t="n">
@@ -10553,7 +10552,7 @@
       </c>
     </row>
     <row r="140" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="5" t="n">
+      <c r="A140" s="4" t="n">
         <v>43661.0833333333</v>
       </c>
       <c r="B140" s="2" t="n">
@@ -10564,7 +10563,7 @@
       </c>
     </row>
     <row r="141" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="5" t="n">
+      <c r="A141" s="4" t="n">
         <v>43658.0833333333</v>
       </c>
       <c r="B141" s="2" t="n">
@@ -10575,7 +10574,7 @@
       </c>
     </row>
     <row r="142" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="5" t="n">
+      <c r="A142" s="4" t="n">
         <v>43657.0833333333</v>
       </c>
       <c r="B142" s="2" t="n">
@@ -10586,7 +10585,7 @@
       </c>
     </row>
     <row r="143" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="5" t="n">
+      <c r="A143" s="4" t="n">
         <v>43656.0833333333</v>
       </c>
       <c r="B143" s="2" t="n">
@@ -10597,7 +10596,7 @@
       </c>
     </row>
     <row r="144" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="5" t="n">
+      <c r="A144" s="4" t="n">
         <v>43655.0833333333</v>
       </c>
       <c r="B144" s="2" t="n">
@@ -10608,7 +10607,7 @@
       </c>
     </row>
     <row r="145" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="5" t="n">
+      <c r="A145" s="4" t="n">
         <v>43654.0833333333</v>
       </c>
       <c r="B145" s="2" t="n">
@@ -10619,7 +10618,7 @@
       </c>
     </row>
     <row r="146" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="5" t="n">
+      <c r="A146" s="4" t="n">
         <v>43651.0833333333</v>
       </c>
       <c r="B146" s="2" t="n">
@@ -10630,7 +10629,7 @@
       </c>
     </row>
     <row r="147" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="5" t="n">
+      <c r="A147" s="4" t="n">
         <v>43650.0833333333</v>
       </c>
       <c r="B147" s="2" t="n">
@@ -10641,7 +10640,7 @@
       </c>
     </row>
     <row r="148" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="5" t="n">
+      <c r="A148" s="4" t="n">
         <v>43649.0833333333</v>
       </c>
       <c r="B148" s="2" t="n">
@@ -10652,7 +10651,7 @@
       </c>
     </row>
     <row r="149" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="5" t="n">
+      <c r="A149" s="4" t="n">
         <v>43648.0833333333</v>
       </c>
       <c r="B149" s="2" t="n">
@@ -10663,7 +10662,7 @@
       </c>
     </row>
     <row r="150" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="5" t="n">
+      <c r="A150" s="4" t="n">
         <v>43647.0833333333</v>
       </c>
       <c r="B150" s="2" t="n">
@@ -10674,7 +10673,7 @@
       </c>
     </row>
     <row r="151" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="5" t="n">
+      <c r="A151" s="4" t="n">
         <v>43644.0833333333</v>
       </c>
       <c r="B151" s="2" t="n">
@@ -10685,7 +10684,7 @@
       </c>
     </row>
     <row r="152" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="5" t="n">
+      <c r="A152" s="4" t="n">
         <v>43643.0833333333</v>
       </c>
       <c r="B152" s="2" t="n">
@@ -10696,7 +10695,7 @@
       </c>
     </row>
     <row r="153" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="5" t="n">
+      <c r="A153" s="4" t="n">
         <v>43642.0833333333</v>
       </c>
       <c r="B153" s="2" t="n">
@@ -10707,7 +10706,7 @@
       </c>
     </row>
     <row r="154" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="5" t="n">
+      <c r="A154" s="4" t="n">
         <v>43641.0833333333</v>
       </c>
       <c r="B154" s="2" t="n">
@@ -10718,7 +10717,7 @@
       </c>
     </row>
     <row r="155" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="5" t="n">
+      <c r="A155" s="4" t="n">
         <v>43640.0833333333</v>
       </c>
       <c r="B155" s="2" t="n">
@@ -10729,7 +10728,7 @@
       </c>
     </row>
     <row r="156" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="5" t="n">
+      <c r="A156" s="4" t="n">
         <v>43637.0833333333</v>
       </c>
       <c r="B156" s="2" t="n">
@@ -10740,7 +10739,7 @@
       </c>
     </row>
     <row r="157" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="5" t="n">
+      <c r="A157" s="4" t="n">
         <v>43636.0833333333</v>
       </c>
       <c r="B157" s="2" t="n">
@@ -10751,7 +10750,7 @@
       </c>
     </row>
     <row r="158" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="5" t="n">
+      <c r="A158" s="4" t="n">
         <v>43635.0833333333</v>
       </c>
       <c r="B158" s="2" t="n">
@@ -10762,7 +10761,7 @@
       </c>
     </row>
     <row r="159" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="5" t="n">
+      <c r="A159" s="4" t="n">
         <v>43634.0833333333</v>
       </c>
       <c r="B159" s="2" t="n">
@@ -10773,7 +10772,7 @@
       </c>
     </row>
     <row r="160" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="5" t="n">
+      <c r="A160" s="4" t="n">
         <v>43633.0833333333</v>
       </c>
       <c r="B160" s="2" t="n">
@@ -10784,7 +10783,7 @@
       </c>
     </row>
     <row r="161" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="5" t="n">
+      <c r="A161" s="4" t="n">
         <v>43630.0833333333</v>
       </c>
       <c r="B161" s="2" t="n">
@@ -10795,7 +10794,7 @@
       </c>
     </row>
     <row r="162" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="5" t="n">
+      <c r="A162" s="4" t="n">
         <v>43629.0833333333</v>
       </c>
       <c r="B162" s="2" t="n">
@@ -10806,7 +10805,7 @@
       </c>
     </row>
     <row r="163" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="5" t="n">
+      <c r="A163" s="4" t="n">
         <v>43628.0833333333</v>
       </c>
       <c r="B163" s="2" t="n">
@@ -10817,7 +10816,7 @@
       </c>
     </row>
     <row r="164" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="5" t="n">
+      <c r="A164" s="4" t="n">
         <v>43627.0833333333</v>
       </c>
       <c r="B164" s="2" t="n">
@@ -10828,7 +10827,7 @@
       </c>
     </row>
     <row r="165" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A165" s="5" t="n">
+      <c r="A165" s="4" t="n">
         <v>43626.0833333333</v>
       </c>
       <c r="B165" s="2" t="n">
@@ -10839,7 +10838,7 @@
       </c>
     </row>
     <row r="166" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="5" t="n">
+      <c r="A166" s="4" t="n">
         <v>43623.0833333333</v>
       </c>
       <c r="B166" s="2" t="n">
@@ -10850,7 +10849,7 @@
       </c>
     </row>
     <row r="167" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="5" t="n">
+      <c r="A167" s="4" t="n">
         <v>43622.0833333333</v>
       </c>
       <c r="B167" s="2" t="n">
@@ -10861,7 +10860,7 @@
       </c>
     </row>
     <row r="168" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A168" s="5" t="n">
+      <c r="A168" s="4" t="n">
         <v>43621.0833333333</v>
       </c>
       <c r="B168" s="2" t="n">
@@ -10872,7 +10871,7 @@
       </c>
     </row>
     <row r="169" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="5" t="n">
+      <c r="A169" s="4" t="n">
         <v>43620.0833333333</v>
       </c>
       <c r="B169" s="2" t="n">
@@ -10883,7 +10882,7 @@
       </c>
     </row>
     <row r="170" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="5" t="n">
+      <c r="A170" s="4" t="n">
         <v>43619.0833333333</v>
       </c>
       <c r="B170" s="2" t="n">
@@ -10894,7 +10893,7 @@
       </c>
     </row>
     <row r="171" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A171" s="5" t="n">
+      <c r="A171" s="4" t="n">
         <v>43616.0833333333</v>
       </c>
       <c r="B171" s="2" t="n">
@@ -10905,7 +10904,7 @@
       </c>
     </row>
     <row r="172" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A172" s="5" t="n">
+      <c r="A172" s="4" t="n">
         <v>43615.0833333333</v>
       </c>
       <c r="B172" s="2" t="n">
@@ -10916,7 +10915,7 @@
       </c>
     </row>
     <row r="173" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A173" s="5" t="n">
+      <c r="A173" s="4" t="n">
         <v>43614.0833333333</v>
       </c>
       <c r="B173" s="2" t="n">
@@ -10927,7 +10926,7 @@
       </c>
     </row>
     <row r="174" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A174" s="5" t="n">
+      <c r="A174" s="4" t="n">
         <v>43613.0833333333</v>
       </c>
       <c r="B174" s="2" t="n">
@@ -10938,7 +10937,7 @@
       </c>
     </row>
     <row r="175" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A175" s="5" t="n">
+      <c r="A175" s="4" t="n">
         <v>43609.0833333333</v>
       </c>
       <c r="B175" s="2" t="n">
@@ -10949,7 +10948,7 @@
       </c>
     </row>
     <row r="176" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A176" s="5" t="n">
+      <c r="A176" s="4" t="n">
         <v>43608.0833333333</v>
       </c>
       <c r="B176" s="2" t="n">
@@ -10960,7 +10959,7 @@
       </c>
     </row>
     <row r="177" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="5" t="n">
+      <c r="A177" s="4" t="n">
         <v>43607.0833333333</v>
       </c>
       <c r="B177" s="2" t="n">
@@ -10971,7 +10970,7 @@
       </c>
     </row>
     <row r="178" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="5" t="n">
+      <c r="A178" s="4" t="n">
         <v>43606.0833333333</v>
       </c>
       <c r="B178" s="2" t="n">
@@ -10982,7 +10981,7 @@
       </c>
     </row>
     <row r="179" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="5" t="n">
+      <c r="A179" s="4" t="n">
         <v>43605.0833333333</v>
       </c>
       <c r="B179" s="2" t="n">
@@ -10993,7 +10992,7 @@
       </c>
     </row>
     <row r="180" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="5" t="n">
+      <c r="A180" s="4" t="n">
         <v>43602.0833333333</v>
       </c>
       <c r="B180" s="2" t="n">
@@ -11004,7 +11003,7 @@
       </c>
     </row>
     <row r="181" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A181" s="5" t="n">
+      <c r="A181" s="4" t="n">
         <v>43601.0833333333</v>
       </c>
       <c r="B181" s="2" t="n">
@@ -11015,7 +11014,7 @@
       </c>
     </row>
     <row r="182" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A182" s="5" t="n">
+      <c r="A182" s="4" t="n">
         <v>43600.0833333333</v>
       </c>
       <c r="B182" s="2" t="n">
@@ -11026,7 +11025,7 @@
       </c>
     </row>
     <row r="183" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A183" s="5" t="n">
+      <c r="A183" s="4" t="n">
         <v>43599.0833333333</v>
       </c>
       <c r="B183" s="2" t="n">
@@ -11037,7 +11036,7 @@
       </c>
     </row>
     <row r="184" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A184" s="5" t="n">
+      <c r="A184" s="4" t="n">
         <v>43598.0833333333</v>
       </c>
       <c r="B184" s="2" t="n">
@@ -11048,7 +11047,7 @@
       </c>
     </row>
     <row r="185" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A185" s="5" t="n">
+      <c r="A185" s="4" t="n">
         <v>43595.0833333333</v>
       </c>
       <c r="B185" s="2" t="n">
@@ -11059,7 +11058,7 @@
       </c>
     </row>
     <row r="186" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A186" s="5" t="n">
+      <c r="A186" s="4" t="n">
         <v>43594.0833333333</v>
       </c>
       <c r="B186" s="2" t="n">
@@ -11070,7 +11069,7 @@
       </c>
     </row>
     <row r="187" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A187" s="5" t="n">
+      <c r="A187" s="4" t="n">
         <v>43593.0833333333</v>
       </c>
       <c r="B187" s="2" t="n">
@@ -11081,7 +11080,7 @@
       </c>
     </row>
     <row r="188" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A188" s="5" t="n">
+      <c r="A188" s="4" t="n">
         <v>43592.0833333333</v>
       </c>
       <c r="B188" s="2" t="n">
@@ -11092,7 +11091,7 @@
       </c>
     </row>
     <row r="189" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A189" s="5" t="n">
+      <c r="A189" s="4" t="n">
         <v>43588.0833333333</v>
       </c>
       <c r="B189" s="2" t="n">
@@ -11103,7 +11102,7 @@
       </c>
     </row>
     <row r="190" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A190" s="5" t="n">
+      <c r="A190" s="4" t="n">
         <v>43587.0833333333</v>
       </c>
       <c r="B190" s="2" t="n">
@@ -11114,7 +11113,7 @@
       </c>
     </row>
     <row r="191" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A191" s="5" t="n">
+      <c r="A191" s="4" t="n">
         <v>43586.0833333333</v>
       </c>
       <c r="B191" s="2" t="n">
@@ -11125,7 +11124,7 @@
       </c>
     </row>
     <row r="192" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A192" s="5" t="n">
+      <c r="A192" s="4" t="n">
         <v>43585.0833333333</v>
       </c>
       <c r="B192" s="2" t="n">
@@ -11136,7 +11135,7 @@
       </c>
     </row>
     <row r="193" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A193" s="5" t="n">
+      <c r="A193" s="4" t="n">
         <v>43584.0833333333</v>
       </c>
       <c r="B193" s="2" t="n">
@@ -11147,7 +11146,7 @@
       </c>
     </row>
     <row r="194" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A194" s="5" t="n">
+      <c r="A194" s="4" t="n">
         <v>43581.0833333333</v>
       </c>
       <c r="B194" s="2" t="n">
@@ -11158,7 +11157,7 @@
       </c>
     </row>
     <row r="195" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A195" s="5" t="n">
+      <c r="A195" s="4" t="n">
         <v>43580.0833333333</v>
       </c>
       <c r="B195" s="2" t="n">
@@ -11169,7 +11168,7 @@
       </c>
     </row>
     <row r="196" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A196" s="5" t="n">
+      <c r="A196" s="4" t="n">
         <v>43579.0833333333</v>
       </c>
       <c r="B196" s="2" t="n">
@@ -11180,7 +11179,7 @@
       </c>
     </row>
     <row r="197" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A197" s="5" t="n">
+      <c r="A197" s="4" t="n">
         <v>43578.0833333333</v>
       </c>
       <c r="B197" s="2" t="n">
@@ -11191,7 +11190,7 @@
       </c>
     </row>
     <row r="198" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A198" s="5" t="n">
+      <c r="A198" s="4" t="n">
         <v>43573.0833333333</v>
       </c>
       <c r="B198" s="2" t="n">
@@ -11202,7 +11201,7 @@
       </c>
     </row>
     <row r="199" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A199" s="5" t="n">
+      <c r="A199" s="4" t="n">
         <v>43572.0833333333</v>
       </c>
       <c r="B199" s="2" t="n">
@@ -11213,7 +11212,7 @@
       </c>
     </row>
     <row r="200" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A200" s="5" t="n">
+      <c r="A200" s="4" t="n">
         <v>43571.0833333333</v>
       </c>
       <c r="B200" s="2" t="n">
@@ -11224,7 +11223,7 @@
       </c>
     </row>
     <row r="201" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A201" s="5" t="n">
+      <c r="A201" s="4" t="n">
         <v>43570.0833333333</v>
       </c>
       <c r="B201" s="2" t="n">
@@ -11235,7 +11234,7 @@
       </c>
     </row>
     <row r="202" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A202" s="5" t="n">
+      <c r="A202" s="4" t="n">
         <v>43567.0833333333</v>
       </c>
       <c r="B202" s="2" t="n">
@@ -11246,7 +11245,7 @@
       </c>
     </row>
     <row r="203" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A203" s="5" t="n">
+      <c r="A203" s="4" t="n">
         <v>43566.0833333333</v>
       </c>
       <c r="B203" s="2" t="n">
@@ -11257,7 +11256,7 @@
       </c>
     </row>
     <row r="204" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A204" s="5" t="n">
+      <c r="A204" s="4" t="n">
         <v>43565.0833333333</v>
       </c>
       <c r="B204" s="2" t="n">
@@ -11268,7 +11267,7 @@
       </c>
     </row>
     <row r="205" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A205" s="5" t="n">
+      <c r="A205" s="4" t="n">
         <v>43564.0833333333</v>
       </c>
       <c r="B205" s="2" t="n">
@@ -11279,7 +11278,7 @@
       </c>
     </row>
     <row r="206" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A206" s="5" t="n">
+      <c r="A206" s="4" t="n">
         <v>43563.0833333333</v>
       </c>
       <c r="B206" s="2" t="n">
@@ -11290,7 +11289,7 @@
       </c>
     </row>
     <row r="207" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A207" s="5" t="n">
+      <c r="A207" s="4" t="n">
         <v>43560.0833333333</v>
       </c>
       <c r="B207" s="2" t="n">
@@ -11301,7 +11300,7 @@
       </c>
     </row>
     <row r="208" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A208" s="5" t="n">
+      <c r="A208" s="4" t="n">
         <v>43559.0833333333</v>
       </c>
       <c r="B208" s="2" t="n">
@@ -11312,7 +11311,7 @@
       </c>
     </row>
     <row r="209" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A209" s="5" t="n">
+      <c r="A209" s="4" t="n">
         <v>43558.0833333333</v>
       </c>
       <c r="B209" s="2" t="n">
@@ -11323,7 +11322,7 @@
       </c>
     </row>
     <row r="210" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A210" s="5" t="n">
+      <c r="A210" s="4" t="n">
         <v>43557.0833333333</v>
       </c>
       <c r="B210" s="2" t="n">
@@ -11334,7 +11333,7 @@
       </c>
     </row>
     <row r="211" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A211" s="5" t="n">
+      <c r="A211" s="4" t="n">
         <v>43556.0833333333</v>
       </c>
       <c r="B211" s="2" t="n">
@@ -11345,7 +11344,7 @@
       </c>
     </row>
     <row r="212" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A212" s="5" t="n">
+      <c r="A212" s="4" t="n">
         <v>43553.0416666667</v>
       </c>
       <c r="B212" s="2" t="n">
@@ -11356,7 +11355,7 @@
       </c>
     </row>
     <row r="213" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A213" s="5" t="n">
+      <c r="A213" s="4" t="n">
         <v>43552.0416666667</v>
       </c>
       <c r="B213" s="2" t="n">
@@ -11367,7 +11366,7 @@
       </c>
     </row>
     <row r="214" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A214" s="5" t="n">
+      <c r="A214" s="4" t="n">
         <v>43551.0416666667</v>
       </c>
       <c r="B214" s="2" t="n">
@@ -11378,7 +11377,7 @@
       </c>
     </row>
     <row r="215" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A215" s="5" t="n">
+      <c r="A215" s="4" t="n">
         <v>43550.0416666667</v>
       </c>
       <c r="B215" s="2" t="n">
@@ -11389,7 +11388,7 @@
       </c>
     </row>
     <row r="216" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A216" s="5" t="n">
+      <c r="A216" s="4" t="n">
         <v>43549.0416666667</v>
       </c>
       <c r="B216" s="2" t="n">
@@ -11400,7 +11399,7 @@
       </c>
     </row>
     <row r="217" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A217" s="5" t="n">
+      <c r="A217" s="4" t="n">
         <v>43546.0416666667</v>
       </c>
       <c r="B217" s="2" t="n">
@@ -11411,7 +11410,7 @@
       </c>
     </row>
     <row r="218" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A218" s="5" t="n">
+      <c r="A218" s="4" t="n">
         <v>43545.0416666667</v>
       </c>
       <c r="B218" s="2" t="n">
@@ -11422,7 +11421,7 @@
       </c>
     </row>
     <row r="219" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A219" s="5" t="n">
+      <c r="A219" s="4" t="n">
         <v>43544.0416666667</v>
       </c>
       <c r="B219" s="2" t="n">
@@ -11433,7 +11432,7 @@
       </c>
     </row>
     <row r="220" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A220" s="5" t="n">
+      <c r="A220" s="4" t="n">
         <v>43543.0416666667</v>
       </c>
       <c r="B220" s="2" t="n">
@@ -11444,7 +11443,7 @@
       </c>
     </row>
     <row r="221" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A221" s="5" t="n">
+      <c r="A221" s="4" t="n">
         <v>43542.0416666667</v>
       </c>
       <c r="B221" s="2" t="n">
@@ -11455,7 +11454,7 @@
       </c>
     </row>
     <row r="222" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A222" s="5" t="n">
+      <c r="A222" s="4" t="n">
         <v>43539.0416666667</v>
       </c>
       <c r="B222" s="2" t="n">
@@ -11466,7 +11465,7 @@
       </c>
     </row>
     <row r="223" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A223" s="5" t="n">
+      <c r="A223" s="4" t="n">
         <v>43538.0416666667</v>
       </c>
       <c r="B223" s="2" t="n">
@@ -11477,7 +11476,7 @@
       </c>
     </row>
     <row r="224" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A224" s="5" t="n">
+      <c r="A224" s="4" t="n">
         <v>43537.0416666667</v>
       </c>
       <c r="B224" s="2" t="n">
@@ -11488,7 +11487,7 @@
       </c>
     </row>
     <row r="225" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A225" s="5" t="n">
+      <c r="A225" s="4" t="n">
         <v>43536.0416666667</v>
       </c>
       <c r="B225" s="2" t="n">
@@ -11499,7 +11498,7 @@
       </c>
     </row>
     <row r="226" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A226" s="5" t="n">
+      <c r="A226" s="4" t="n">
         <v>43535.0416666667</v>
       </c>
       <c r="B226" s="2" t="n">
@@ -11510,7 +11509,7 @@
       </c>
     </row>
     <row r="227" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A227" s="5" t="n">
+      <c r="A227" s="4" t="n">
         <v>43532.0416666667</v>
       </c>
       <c r="B227" s="2" t="n">
@@ -11521,7 +11520,7 @@
       </c>
     </row>
     <row r="228" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A228" s="5" t="n">
+      <c r="A228" s="4" t="n">
         <v>43531.0416666667</v>
       </c>
       <c r="B228" s="2" t="n">
@@ -11532,7 +11531,7 @@
       </c>
     </row>
     <row r="229" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A229" s="5" t="n">
+      <c r="A229" s="4" t="n">
         <v>43530.0416666667</v>
       </c>
       <c r="B229" s="2" t="n">
@@ -11543,7 +11542,7 @@
       </c>
     </row>
     <row r="230" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A230" s="5" t="n">
+      <c r="A230" s="4" t="n">
         <v>43529.0416666667</v>
       </c>
       <c r="B230" s="2" t="n">
@@ -11554,7 +11553,7 @@
       </c>
     </row>
     <row r="231" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A231" s="5" t="n">
+      <c r="A231" s="4" t="n">
         <v>43528.0416666667</v>
       </c>
       <c r="B231" s="2" t="n">
@@ -11565,7 +11564,7 @@
       </c>
     </row>
     <row r="232" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A232" s="5" t="n">
+      <c r="A232" s="4" t="n">
         <v>43525.0416666667</v>
       </c>
       <c r="B232" s="2" t="n">
@@ -11576,7 +11575,7 @@
       </c>
     </row>
     <row r="233" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A233" s="5" t="n">
+      <c r="A233" s="4" t="n">
         <v>43524.0416666667</v>
       </c>
       <c r="B233" s="2" t="n">
@@ -11587,7 +11586,7 @@
       </c>
     </row>
     <row r="234" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A234" s="5" t="n">
+      <c r="A234" s="4" t="n">
         <v>43523.0416666667</v>
       </c>
       <c r="B234" s="2" t="n">
@@ -11598,7 +11597,7 @@
       </c>
     </row>
     <row r="235" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A235" s="5" t="n">
+      <c r="A235" s="4" t="n">
         <v>43522.0416666667</v>
       </c>
       <c r="B235" s="2" t="n">
@@ -11609,7 +11608,7 @@
       </c>
     </row>
     <row r="236" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A236" s="5" t="n">
+      <c r="A236" s="4" t="n">
         <v>43521.0416666667</v>
       </c>
       <c r="B236" s="2" t="n">
@@ -11620,7 +11619,7 @@
       </c>
     </row>
     <row r="237" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A237" s="5" t="n">
+      <c r="A237" s="4" t="n">
         <v>43518.0416666667</v>
       </c>
       <c r="B237" s="2" t="n">
@@ -11631,7 +11630,7 @@
       </c>
     </row>
     <row r="238" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A238" s="5" t="n">
+      <c r="A238" s="4" t="n">
         <v>43517.0416666667</v>
       </c>
       <c r="B238" s="2" t="n">
@@ -11642,7 +11641,7 @@
       </c>
     </row>
     <row r="239" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A239" s="5" t="n">
+      <c r="A239" s="4" t="n">
         <v>43516.0416666667</v>
       </c>
       <c r="B239" s="2" t="n">
@@ -11653,7 +11652,7 @@
       </c>
     </row>
     <row r="240" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A240" s="5" t="n">
+      <c r="A240" s="4" t="n">
         <v>43515.0416666667</v>
       </c>
       <c r="B240" s="2" t="n">
@@ -11664,7 +11663,7 @@
       </c>
     </row>
     <row r="241" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A241" s="5" t="n">
+      <c r="A241" s="4" t="n">
         <v>43514.0416666667</v>
       </c>
       <c r="B241" s="2" t="n">
@@ -11675,7 +11674,7 @@
       </c>
     </row>
     <row r="242" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A242" s="5" t="n">
+      <c r="A242" s="4" t="n">
         <v>43511.0416666667</v>
       </c>
       <c r="B242" s="2" t="n">
@@ -11686,7 +11685,7 @@
       </c>
     </row>
     <row r="243" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A243" s="5" t="n">
+      <c r="A243" s="4" t="n">
         <v>43510.0416666667</v>
       </c>
       <c r="B243" s="2" t="n">
@@ -11697,7 +11696,7 @@
       </c>
     </row>
     <row r="244" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A244" s="5" t="n">
+      <c r="A244" s="4" t="n">
         <v>43509.0416666667</v>
       </c>
       <c r="B244" s="2" t="n">
@@ -11708,7 +11707,7 @@
       </c>
     </row>
     <row r="245" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A245" s="5" t="n">
+      <c r="A245" s="4" t="n">
         <v>43508.0416666667</v>
       </c>
       <c r="B245" s="2" t="n">
@@ -11719,7 +11718,7 @@
       </c>
     </row>
     <row r="246" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A246" s="5" t="n">
+      <c r="A246" s="4" t="n">
         <v>43507.0416666667</v>
       </c>
       <c r="B246" s="2" t="n">
@@ -11730,7 +11729,7 @@
       </c>
     </row>
     <row r="247" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A247" s="5" t="n">
+      <c r="A247" s="4" t="n">
         <v>43504.0416666667</v>
       </c>
       <c r="B247" s="2" t="n">
@@ -11741,7 +11740,7 @@
       </c>
     </row>
     <row r="248" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A248" s="5" t="n">
+      <c r="A248" s="4" t="n">
         <v>43503.0416666667</v>
       </c>
       <c r="B248" s="2" t="n">
@@ -11752,7 +11751,7 @@
       </c>
     </row>
     <row r="249" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A249" s="5" t="n">
+      <c r="A249" s="4" t="n">
         <v>43502.0416666667</v>
       </c>
       <c r="B249" s="2" t="n">
@@ -11763,7 +11762,7 @@
       </c>
     </row>
     <row r="250" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A250" s="5" t="n">
+      <c r="A250" s="4" t="n">
         <v>43501.0416666667</v>
       </c>
       <c r="B250" s="2" t="n">
@@ -11774,7 +11773,7 @@
       </c>
     </row>
     <row r="251" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A251" s="5" t="n">
+      <c r="A251" s="4" t="n">
         <v>43500.0416666667</v>
       </c>
       <c r="B251" s="2" t="n">
@@ -11785,7 +11784,7 @@
       </c>
     </row>
     <row r="252" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A252" s="5" t="n">
+      <c r="A252" s="4" t="n">
         <v>43497.0416666667</v>
       </c>
       <c r="B252" s="2" t="n">
@@ -11796,7 +11795,7 @@
       </c>
     </row>
     <row r="253" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A253" s="5" t="n">
+      <c r="A253" s="4" t="n">
         <v>43496.0416666667</v>
       </c>
       <c r="B253" s="2" t="n">
@@ -11807,7 +11806,7 @@
       </c>
     </row>
     <row r="254" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A254" s="5" t="n">
+      <c r="A254" s="4" t="n">
         <v>43495.0416666667</v>
       </c>
       <c r="B254" s="2" t="n">
@@ -11817,8 +11816,8 @@
         <v>128.73</v>
       </c>
     </row>
-    <row r="255" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A255" s="5" t="n">
+    <row r="255" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A255" s="4" t="n">
         <v>43494.0416666667</v>
       </c>
       <c r="B255" s="2" t="n">
@@ -11846,8 +11845,8 @@
   </sheetPr>
   <dimension ref="A1:C255"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A:A"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11858,7 +11857,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>185</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -11869,7 +11868,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="n">
+      <c r="A2" s="4" t="n">
         <v>43859.0416666667</v>
       </c>
       <c r="B2" s="2" t="n">
@@ -11880,7 +11879,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="n">
+      <c r="A3" s="4" t="n">
         <v>43858.0416666667</v>
       </c>
       <c r="B3" s="2" t="n">
@@ -11891,7 +11890,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="n">
+      <c r="A4" s="4" t="n">
         <v>43857.0416666667</v>
       </c>
       <c r="B4" s="2" t="n">
@@ -11902,7 +11901,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="n">
+      <c r="A5" s="4" t="n">
         <v>43854.0416666667</v>
       </c>
       <c r="B5" s="2" t="n">
@@ -11913,7 +11912,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="n">
+      <c r="A6" s="4" t="n">
         <v>43853.0416666667</v>
       </c>
       <c r="B6" s="2" t="n">
@@ -11924,7 +11923,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="n">
+      <c r="A7" s="4" t="n">
         <v>43852.0416666667</v>
       </c>
       <c r="B7" s="2" t="n">
@@ -11935,7 +11934,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="n">
+      <c r="A8" s="4" t="n">
         <v>43851.0416666667</v>
       </c>
       <c r="B8" s="2" t="n">
@@ -11946,7 +11945,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="n">
+      <c r="A9" s="4" t="n">
         <v>43850.0416666667</v>
       </c>
       <c r="B9" s="2" t="n">
@@ -11957,7 +11956,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="n">
+      <c r="A10" s="4" t="n">
         <v>43847.0416666667</v>
       </c>
       <c r="B10" s="2" t="n">
@@ -11968,7 +11967,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="n">
+      <c r="A11" s="4" t="n">
         <v>43846.0416666667</v>
       </c>
       <c r="B11" s="2" t="n">
@@ -11979,7 +11978,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="n">
+      <c r="A12" s="4" t="n">
         <v>43845.0416666667</v>
       </c>
       <c r="B12" s="2" t="n">
@@ -11990,7 +11989,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="n">
+      <c r="A13" s="4" t="n">
         <v>43844.0416666667</v>
       </c>
       <c r="B13" s="2" t="n">
@@ -12001,7 +12000,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="n">
+      <c r="A14" s="4" t="n">
         <v>43843.0416666667</v>
       </c>
       <c r="B14" s="2" t="n">
@@ -12012,7 +12011,7 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="n">
+      <c r="A15" s="4" t="n">
         <v>43840.0416666667</v>
       </c>
       <c r="B15" s="2" t="n">
@@ -12023,7 +12022,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5" t="n">
+      <c r="A16" s="4" t="n">
         <v>43839.0416666667</v>
       </c>
       <c r="B16" s="2" t="n">
@@ -12034,7 +12033,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5" t="n">
+      <c r="A17" s="4" t="n">
         <v>43838.0416666667</v>
       </c>
       <c r="B17" s="2" t="n">
@@ -12045,7 +12044,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5" t="n">
+      <c r="A18" s="4" t="n">
         <v>43837.0416666667</v>
       </c>
       <c r="B18" s="2" t="n">
@@ -12056,7 +12055,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5" t="n">
+      <c r="A19" s="4" t="n">
         <v>43836.0416666667</v>
       </c>
       <c r="B19" s="2" t="n">
@@ -12067,7 +12066,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5" t="n">
+      <c r="A20" s="4" t="n">
         <v>43833.0416666667</v>
       </c>
       <c r="B20" s="2" t="n">
@@ -12078,7 +12077,7 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="5" t="n">
+      <c r="A21" s="4" t="n">
         <v>43832.0416666667</v>
       </c>
       <c r="B21" s="2" t="n">
@@ -12089,7 +12088,7 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="5" t="n">
+      <c r="A22" s="4" t="n">
         <v>43830.0416666667</v>
       </c>
       <c r="B22" s="2" t="n">
@@ -12100,7 +12099,7 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="5" t="n">
+      <c r="A23" s="4" t="n">
         <v>43829.0416666667</v>
       </c>
       <c r="B23" s="2" t="n">
@@ -12111,7 +12110,7 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="5" t="n">
+      <c r="A24" s="4" t="n">
         <v>43826.0416666667</v>
       </c>
       <c r="B24" s="2" t="n">
@@ -12122,7 +12121,7 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="5" t="n">
+      <c r="A25" s="4" t="n">
         <v>43823.0416666667</v>
       </c>
       <c r="B25" s="2" t="n">
@@ -12133,7 +12132,7 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="5" t="n">
+      <c r="A26" s="4" t="n">
         <v>43822.0416666667</v>
       </c>
       <c r="B26" s="2" t="n">
@@ -12144,7 +12143,7 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="5" t="n">
+      <c r="A27" s="4" t="n">
         <v>43819.0416666667</v>
       </c>
       <c r="B27" s="2" t="n">
@@ -12155,7 +12154,7 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="5" t="n">
+      <c r="A28" s="4" t="n">
         <v>43818.0416666667</v>
       </c>
       <c r="B28" s="2" t="n">
@@ -12166,7 +12165,7 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="5" t="n">
+      <c r="A29" s="4" t="n">
         <v>43817.0416666667</v>
       </c>
       <c r="B29" s="2" t="n">
@@ -12177,7 +12176,7 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="5" t="n">
+      <c r="A30" s="4" t="n">
         <v>43816.0416666667</v>
       </c>
       <c r="B30" s="2" t="n">
@@ -12188,7 +12187,7 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="5" t="n">
+      <c r="A31" s="4" t="n">
         <v>43815.0416666667</v>
       </c>
       <c r="B31" s="2" t="n">
@@ -12199,7 +12198,7 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="5" t="n">
+      <c r="A32" s="4" t="n">
         <v>43812.0416666667</v>
       </c>
       <c r="B32" s="2" t="n">
@@ -12210,7 +12209,7 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="5" t="n">
+      <c r="A33" s="4" t="n">
         <v>43811.0416666667</v>
       </c>
       <c r="B33" s="2" t="n">
@@ -12221,7 +12220,7 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="5" t="n">
+      <c r="A34" s="4" t="n">
         <v>43810.0416666667</v>
       </c>
       <c r="B34" s="2" t="n">
@@ -12232,7 +12231,7 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="5" t="n">
+      <c r="A35" s="4" t="n">
         <v>43809.0416666667</v>
       </c>
       <c r="B35" s="2" t="n">
@@ -12243,7 +12242,7 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="5" t="n">
+      <c r="A36" s="4" t="n">
         <v>43808.0416666667</v>
       </c>
       <c r="B36" s="2" t="n">
@@ -12254,7 +12253,7 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="5" t="n">
+      <c r="A37" s="4" t="n">
         <v>43805.0416666667</v>
       </c>
       <c r="B37" s="2" t="n">
@@ -12265,7 +12264,7 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="5" t="n">
+      <c r="A38" s="4" t="n">
         <v>43804.0416666667</v>
       </c>
       <c r="B38" s="2" t="n">
@@ -12276,7 +12275,7 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="5" t="n">
+      <c r="A39" s="4" t="n">
         <v>43803.0416666667</v>
       </c>
       <c r="B39" s="2" t="n">
@@ -12287,7 +12286,7 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="5" t="n">
+      <c r="A40" s="4" t="n">
         <v>43802.0416666667</v>
       </c>
       <c r="B40" s="2" t="n">
@@ -12298,7 +12297,7 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="5" t="n">
+      <c r="A41" s="4" t="n">
         <v>43801.0416666667</v>
       </c>
       <c r="B41" s="2" t="n">
@@ -12309,7 +12308,7 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="5" t="n">
+      <c r="A42" s="4" t="n">
         <v>43798.0416666667</v>
       </c>
       <c r="B42" s="2" t="n">
@@ -12320,7 +12319,7 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="5" t="n">
+      <c r="A43" s="4" t="n">
         <v>43797.0416666667</v>
       </c>
       <c r="B43" s="2" t="n">
@@ -12331,7 +12330,7 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="5" t="n">
+      <c r="A44" s="4" t="n">
         <v>43796.0416666667</v>
       </c>
       <c r="B44" s="2" t="n">
@@ -12342,7 +12341,7 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="5" t="n">
+      <c r="A45" s="4" t="n">
         <v>43795.0416666667</v>
       </c>
       <c r="B45" s="2" t="n">
@@ -12353,7 +12352,7 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="5" t="n">
+      <c r="A46" s="4" t="n">
         <v>43794.0416666667</v>
       </c>
       <c r="B46" s="2" t="n">
@@ -12364,7 +12363,7 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="5" t="n">
+      <c r="A47" s="4" t="n">
         <v>43791.0416666667</v>
       </c>
       <c r="B47" s="2" t="n">
@@ -12375,7 +12374,7 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="5" t="n">
+      <c r="A48" s="4" t="n">
         <v>43790.0416666667</v>
       </c>
       <c r="B48" s="2" t="n">
@@ -12386,7 +12385,7 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="5" t="n">
+      <c r="A49" s="4" t="n">
         <v>43789.0416666667</v>
       </c>
       <c r="B49" s="2" t="n">
@@ -12397,7 +12396,7 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="5" t="n">
+      <c r="A50" s="4" t="n">
         <v>43788.0416666667</v>
       </c>
       <c r="B50" s="2" t="n">
@@ -12408,7 +12407,7 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="5" t="n">
+      <c r="A51" s="4" t="n">
         <v>43787.0416666667</v>
       </c>
       <c r="B51" s="2" t="n">
@@ -12419,7 +12418,7 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="5" t="n">
+      <c r="A52" s="4" t="n">
         <v>43784.0416666667</v>
       </c>
       <c r="B52" s="2" t="n">
@@ -12430,7 +12429,7 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="5" t="n">
+      <c r="A53" s="4" t="n">
         <v>43783.0416666667</v>
       </c>
       <c r="B53" s="2" t="n">
@@ -12441,7 +12440,7 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="5" t="n">
+      <c r="A54" s="4" t="n">
         <v>43782.0416666667</v>
       </c>
       <c r="B54" s="2" t="n">
@@ -12452,7 +12451,7 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="5" t="n">
+      <c r="A55" s="4" t="n">
         <v>43781.0416666667</v>
       </c>
       <c r="B55" s="2" t="n">
@@ -12463,7 +12462,7 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="5" t="n">
+      <c r="A56" s="4" t="n">
         <v>43780.0416666667</v>
       </c>
       <c r="B56" s="2" t="n">
@@ -12474,7 +12473,7 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="5" t="n">
+      <c r="A57" s="4" t="n">
         <v>43777.0416666667</v>
       </c>
       <c r="B57" s="2" t="n">
@@ -12485,7 +12484,7 @@
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="5" t="n">
+      <c r="A58" s="4" t="n">
         <v>43776.0416666667</v>
       </c>
       <c r="B58" s="2" t="n">
@@ -12496,7 +12495,7 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="5" t="n">
+      <c r="A59" s="4" t="n">
         <v>43775.0416666667</v>
       </c>
       <c r="B59" s="2" t="n">
@@ -12507,7 +12506,7 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="5" t="n">
+      <c r="A60" s="4" t="n">
         <v>43774.0416666667</v>
       </c>
       <c r="B60" s="2" t="n">
@@ -12518,7 +12517,7 @@
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="5" t="n">
+      <c r="A61" s="4" t="n">
         <v>43773.0416666667</v>
       </c>
       <c r="B61" s="2" t="n">
@@ -12529,7 +12528,7 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="5" t="n">
+      <c r="A62" s="4" t="n">
         <v>43770.0416666667</v>
       </c>
       <c r="B62" s="2" t="n">
@@ -12540,7 +12539,7 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="5" t="n">
+      <c r="A63" s="4" t="n">
         <v>43769.0416666667</v>
       </c>
       <c r="B63" s="2" t="n">
@@ -12551,7 +12550,7 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="5" t="n">
+      <c r="A64" s="4" t="n">
         <v>43768.0416666667</v>
       </c>
       <c r="B64" s="2" t="n">
@@ -12562,7 +12561,7 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="5" t="n">
+      <c r="A65" s="4" t="n">
         <v>43767.0416666667</v>
       </c>
       <c r="B65" s="2" t="n">
@@ -12573,7 +12572,7 @@
       </c>
     </row>
     <row r="66" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="5" t="n">
+      <c r="A66" s="4" t="n">
         <v>43766.0416666667</v>
       </c>
       <c r="B66" s="2" t="n">
@@ -12584,7 +12583,7 @@
       </c>
     </row>
     <row r="67" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="5" t="n">
+      <c r="A67" s="4" t="n">
         <v>43763.0833333333</v>
       </c>
       <c r="B67" s="2" t="n">
@@ -12595,7 +12594,7 @@
       </c>
     </row>
     <row r="68" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="5" t="n">
+      <c r="A68" s="4" t="n">
         <v>43762.0833333333</v>
       </c>
       <c r="B68" s="2" t="n">
@@ -12606,7 +12605,7 @@
       </c>
     </row>
     <row r="69" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="5" t="n">
+      <c r="A69" s="4" t="n">
         <v>43761.0833333333</v>
       </c>
       <c r="B69" s="2" t="n">
@@ -12617,7 +12616,7 @@
       </c>
     </row>
     <row r="70" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="5" t="n">
+      <c r="A70" s="4" t="n">
         <v>43760.0833333333</v>
       </c>
       <c r="B70" s="2" t="n">
@@ -12628,7 +12627,7 @@
       </c>
     </row>
     <row r="71" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="5" t="n">
+      <c r="A71" s="4" t="n">
         <v>43759.0833333333</v>
       </c>
       <c r="B71" s="2" t="n">
@@ -12639,7 +12638,7 @@
       </c>
     </row>
     <row r="72" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="5" t="n">
+      <c r="A72" s="4" t="n">
         <v>43756.0833333333</v>
       </c>
       <c r="B72" s="2" t="n">
@@ -12650,7 +12649,7 @@
       </c>
     </row>
     <row r="73" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="5" t="n">
+      <c r="A73" s="4" t="n">
         <v>43755.0833333333</v>
       </c>
       <c r="B73" s="2" t="n">
@@ -12661,7 +12660,7 @@
       </c>
     </row>
     <row r="74" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="5" t="n">
+      <c r="A74" s="4" t="n">
         <v>43754.0833333333</v>
       </c>
       <c r="B74" s="2" t="n">
@@ -12672,7 +12671,7 @@
       </c>
     </row>
     <row r="75" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="5" t="n">
+      <c r="A75" s="4" t="n">
         <v>43753.0833333333</v>
       </c>
       <c r="B75" s="2" t="n">
@@ -12683,7 +12682,7 @@
       </c>
     </row>
     <row r="76" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="5" t="n">
+      <c r="A76" s="4" t="n">
         <v>43752.0833333333</v>
       </c>
       <c r="B76" s="2" t="n">
@@ -12694,7 +12693,7 @@
       </c>
     </row>
     <row r="77" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="5" t="n">
+      <c r="A77" s="4" t="n">
         <v>43749.0833333333</v>
       </c>
       <c r="B77" s="2" t="n">
@@ -12705,7 +12704,7 @@
       </c>
     </row>
     <row r="78" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="5" t="n">
+      <c r="A78" s="4" t="n">
         <v>43748.0833333333</v>
       </c>
       <c r="B78" s="2" t="n">
@@ -12716,7 +12715,7 @@
       </c>
     </row>
     <row r="79" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="5" t="n">
+      <c r="A79" s="4" t="n">
         <v>43747.0833333333</v>
       </c>
       <c r="B79" s="2" t="n">
@@ -12727,7 +12726,7 @@
       </c>
     </row>
     <row r="80" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="5" t="n">
+      <c r="A80" s="4" t="n">
         <v>43746.0833333333</v>
       </c>
       <c r="B80" s="2" t="n">
@@ -12738,7 +12737,7 @@
       </c>
     </row>
     <row r="81" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="5" t="n">
+      <c r="A81" s="4" t="n">
         <v>43745.0833333333</v>
       </c>
       <c r="B81" s="2" t="n">
@@ -12749,7 +12748,7 @@
       </c>
     </row>
     <row r="82" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="5" t="n">
+      <c r="A82" s="4" t="n">
         <v>43742.0833333333</v>
       </c>
       <c r="B82" s="2" t="n">
@@ -12760,7 +12759,7 @@
       </c>
     </row>
     <row r="83" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="5" t="n">
+      <c r="A83" s="4" t="n">
         <v>43741.0833333333</v>
       </c>
       <c r="B83" s="2" t="n">
@@ -12771,7 +12770,7 @@
       </c>
     </row>
     <row r="84" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="5" t="n">
+      <c r="A84" s="4" t="n">
         <v>43740.0833333333</v>
       </c>
       <c r="B84" s="2" t="n">
@@ -12782,7 +12781,7 @@
       </c>
     </row>
     <row r="85" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="5" t="n">
+      <c r="A85" s="4" t="n">
         <v>43739.0833333333</v>
       </c>
       <c r="B85" s="2" t="n">
@@ -12793,7 +12792,7 @@
       </c>
     </row>
     <row r="86" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="5" t="n">
+      <c r="A86" s="4" t="n">
         <v>43738.0833333333</v>
       </c>
       <c r="B86" s="2" t="n">
@@ -12804,7 +12803,7 @@
       </c>
     </row>
     <row r="87" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="5" t="n">
+      <c r="A87" s="4" t="n">
         <v>43735.0833333333</v>
       </c>
       <c r="B87" s="2" t="n">
@@ -12815,7 +12814,7 @@
       </c>
     </row>
     <row r="88" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="5" t="n">
+      <c r="A88" s="4" t="n">
         <v>43734.0833333333</v>
       </c>
       <c r="B88" s="2" t="n">
@@ -12826,7 +12825,7 @@
       </c>
     </row>
     <row r="89" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="5" t="n">
+      <c r="A89" s="4" t="n">
         <v>43733.0833333333</v>
       </c>
       <c r="B89" s="2" t="n">
@@ -12837,7 +12836,7 @@
       </c>
     </row>
     <row r="90" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="5" t="n">
+      <c r="A90" s="4" t="n">
         <v>43732.0833333333</v>
       </c>
       <c r="B90" s="2" t="n">
@@ -12848,7 +12847,7 @@
       </c>
     </row>
     <row r="91" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="5" t="n">
+      <c r="A91" s="4" t="n">
         <v>43731.0833333333</v>
       </c>
       <c r="B91" s="2" t="n">
@@ -12859,7 +12858,7 @@
       </c>
     </row>
     <row r="92" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="5" t="n">
+      <c r="A92" s="4" t="n">
         <v>43728.0833333333</v>
       </c>
       <c r="B92" s="2" t="n">
@@ -12870,7 +12869,7 @@
       </c>
     </row>
     <row r="93" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="5" t="n">
+      <c r="A93" s="4" t="n">
         <v>43727.0833333333</v>
       </c>
       <c r="B93" s="2" t="n">
@@ -12881,7 +12880,7 @@
       </c>
     </row>
     <row r="94" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="5" t="n">
+      <c r="A94" s="4" t="n">
         <v>43726.0833333333</v>
       </c>
       <c r="B94" s="2" t="n">
@@ -12892,7 +12891,7 @@
       </c>
     </row>
     <row r="95" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="5" t="n">
+      <c r="A95" s="4" t="n">
         <v>43725.0833333333</v>
       </c>
       <c r="B95" s="2" t="n">
@@ -12903,7 +12902,7 @@
       </c>
     </row>
     <row r="96" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="5" t="n">
+      <c r="A96" s="4" t="n">
         <v>43724.0833333333</v>
       </c>
       <c r="B96" s="2" t="n">
@@ -12914,7 +12913,7 @@
       </c>
     </row>
     <row r="97" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="5" t="n">
+      <c r="A97" s="4" t="n">
         <v>43721.0833333333</v>
       </c>
       <c r="B97" s="2" t="n">
@@ -12925,7 +12924,7 @@
       </c>
     </row>
     <row r="98" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="5" t="n">
+      <c r="A98" s="4" t="n">
         <v>43720.0833333333</v>
       </c>
       <c r="B98" s="2" t="n">
@@ -12936,7 +12935,7 @@
       </c>
     </row>
     <row r="99" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="5" t="n">
+      <c r="A99" s="4" t="n">
         <v>43719.0833333333</v>
       </c>
       <c r="B99" s="2" t="n">
@@ -12947,7 +12946,7 @@
       </c>
     </row>
     <row r="100" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="5" t="n">
+      <c r="A100" s="4" t="n">
         <v>43718.0833333333</v>
       </c>
       <c r="B100" s="2" t="n">
@@ -12958,7 +12957,7 @@
       </c>
     </row>
     <row r="101" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="5" t="n">
+      <c r="A101" s="4" t="n">
         <v>43717.0833333333</v>
       </c>
       <c r="B101" s="2" t="n">
@@ -12969,7 +12968,7 @@
       </c>
     </row>
     <row r="102" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="5" t="n">
+      <c r="A102" s="4" t="n">
         <v>43714.0833333333</v>
       </c>
       <c r="B102" s="2" t="n">
@@ -12980,7 +12979,7 @@
       </c>
     </row>
     <row r="103" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="5" t="n">
+      <c r="A103" s="4" t="n">
         <v>43713.0833333333</v>
       </c>
       <c r="B103" s="2" t="n">
@@ -12991,7 +12990,7 @@
       </c>
     </row>
     <row r="104" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="5" t="n">
+      <c r="A104" s="4" t="n">
         <v>43712.0833333333</v>
       </c>
       <c r="B104" s="2" t="n">
@@ -13002,7 +13001,7 @@
       </c>
     </row>
     <row r="105" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="5" t="n">
+      <c r="A105" s="4" t="n">
         <v>43711.0833333333</v>
       </c>
       <c r="B105" s="2" t="n">
@@ -13013,7 +13012,7 @@
       </c>
     </row>
     <row r="106" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="5" t="n">
+      <c r="A106" s="4" t="n">
         <v>43710.0833333333</v>
       </c>
       <c r="B106" s="2" t="n">
@@ -13024,7 +13023,7 @@
       </c>
     </row>
     <row r="107" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="5" t="n">
+      <c r="A107" s="4" t="n">
         <v>43707.0833333333</v>
       </c>
       <c r="B107" s="2" t="n">
@@ -13035,7 +13034,7 @@
       </c>
     </row>
     <row r="108" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="5" t="n">
+      <c r="A108" s="4" t="n">
         <v>43706.0833333333</v>
       </c>
       <c r="B108" s="2" t="n">
@@ -13046,7 +13045,7 @@
       </c>
     </row>
     <row r="109" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="5" t="n">
+      <c r="A109" s="4" t="n">
         <v>43705.0833333333</v>
       </c>
       <c r="B109" s="2" t="n">
@@ -13057,7 +13056,7 @@
       </c>
     </row>
     <row r="110" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="5" t="n">
+      <c r="A110" s="4" t="n">
         <v>43704.0833333333</v>
       </c>
       <c r="B110" s="2" t="n">
@@ -13068,7 +13067,7 @@
       </c>
     </row>
     <row r="111" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="5" t="n">
+      <c r="A111" s="4" t="n">
         <v>43700.0833333333</v>
       </c>
       <c r="B111" s="2" t="n">
@@ -13079,7 +13078,7 @@
       </c>
     </row>
     <row r="112" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="5" t="n">
+      <c r="A112" s="4" t="n">
         <v>43699.0833333333</v>
       </c>
       <c r="B112" s="2" t="n">
@@ -13090,7 +13089,7 @@
       </c>
     </row>
     <row r="113" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="5" t="n">
+      <c r="A113" s="4" t="n">
         <v>43698.0833333333</v>
       </c>
       <c r="B113" s="2" t="n">
@@ -13101,7 +13100,7 @@
       </c>
     </row>
     <row r="114" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="5" t="n">
+      <c r="A114" s="4" t="n">
         <v>43697.0833333333</v>
       </c>
       <c r="B114" s="2" t="n">
@@ -13112,7 +13111,7 @@
       </c>
     </row>
     <row r="115" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="5" t="n">
+      <c r="A115" s="4" t="n">
         <v>43696.0833333333</v>
       </c>
       <c r="B115" s="2" t="n">
@@ -13123,7 +13122,7 @@
       </c>
     </row>
     <row r="116" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="5" t="n">
+      <c r="A116" s="4" t="n">
         <v>43693.0833333333</v>
       </c>
       <c r="B116" s="2" t="n">
@@ -13134,7 +13133,7 @@
       </c>
     </row>
     <row r="117" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="5" t="n">
+      <c r="A117" s="4" t="n">
         <v>43692.0833333333</v>
       </c>
       <c r="B117" s="2" t="n">
@@ -13145,7 +13144,7 @@
       </c>
     </row>
     <row r="118" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="5" t="n">
+      <c r="A118" s="4" t="n">
         <v>43691.0833333333</v>
       </c>
       <c r="B118" s="2" t="n">
@@ -13156,7 +13155,7 @@
       </c>
     </row>
     <row r="119" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="5" t="n">
+      <c r="A119" s="4" t="n">
         <v>43690.0833333333</v>
       </c>
       <c r="B119" s="2" t="n">
@@ -13167,7 +13166,7 @@
       </c>
     </row>
     <row r="120" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="5" t="n">
+      <c r="A120" s="4" t="n">
         <v>43689.0833333333</v>
       </c>
       <c r="B120" s="2" t="n">
@@ -13178,7 +13177,7 @@
       </c>
     </row>
     <row r="121" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="5" t="n">
+      <c r="A121" s="4" t="n">
         <v>43686.0833333333</v>
       </c>
       <c r="B121" s="2" t="n">
@@ -13189,7 +13188,7 @@
       </c>
     </row>
     <row r="122" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="5" t="n">
+      <c r="A122" s="4" t="n">
         <v>43685.0833333333</v>
       </c>
       <c r="B122" s="2" t="n">
@@ -13200,7 +13199,7 @@
       </c>
     </row>
     <row r="123" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="5" t="n">
+      <c r="A123" s="4" t="n">
         <v>43684.0833333333</v>
       </c>
       <c r="B123" s="2" t="n">
@@ -13211,7 +13210,7 @@
       </c>
     </row>
     <row r="124" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="5" t="n">
+      <c r="A124" s="4" t="n">
         <v>43683.0833333333</v>
       </c>
       <c r="B124" s="2" t="n">
@@ -13222,7 +13221,7 @@
       </c>
     </row>
     <row r="125" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="5" t="n">
+      <c r="A125" s="4" t="n">
         <v>43682.0833333333</v>
       </c>
       <c r="B125" s="2" t="n">
@@ -13233,7 +13232,7 @@
       </c>
     </row>
     <row r="126" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="5" t="n">
+      <c r="A126" s="4" t="n">
         <v>43679.0833333333</v>
       </c>
       <c r="B126" s="2" t="n">
@@ -13244,7 +13243,7 @@
       </c>
     </row>
     <row r="127" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="5" t="n">
+      <c r="A127" s="4" t="n">
         <v>43678.0833333333</v>
       </c>
       <c r="B127" s="2" t="n">
@@ -13255,7 +13254,7 @@
       </c>
     </row>
     <row r="128" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="5" t="n">
+      <c r="A128" s="4" t="n">
         <v>43677.0833333333</v>
       </c>
       <c r="B128" s="2" t="n">
@@ -13266,7 +13265,7 @@
       </c>
     </row>
     <row r="129" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="5" t="n">
+      <c r="A129" s="4" t="n">
         <v>43676.0833333333</v>
       </c>
       <c r="B129" s="2" t="n">
@@ -13277,7 +13276,7 @@
       </c>
     </row>
     <row r="130" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="5" t="n">
+      <c r="A130" s="4" t="n">
         <v>43675.0833333333</v>
       </c>
       <c r="B130" s="2" t="n">
@@ -13288,7 +13287,7 @@
       </c>
     </row>
     <row r="131" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="5" t="n">
+      <c r="A131" s="4" t="n">
         <v>43672.0833333333</v>
       </c>
       <c r="B131" s="2" t="n">
@@ -13299,7 +13298,7 @@
       </c>
     </row>
     <row r="132" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="5" t="n">
+      <c r="A132" s="4" t="n">
         <v>43671.0833333333</v>
       </c>
       <c r="B132" s="2" t="n">
@@ -13310,7 +13309,7 @@
       </c>
     </row>
     <row r="133" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="5" t="n">
+      <c r="A133" s="4" t="n">
         <v>43670.0833333333</v>
       </c>
       <c r="B133" s="2" t="n">
@@ -13321,7 +13320,7 @@
       </c>
     </row>
     <row r="134" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="5" t="n">
+      <c r="A134" s="4" t="n">
         <v>43669.0833333333</v>
       </c>
       <c r="B134" s="2" t="n">
@@ -13332,7 +13331,7 @@
       </c>
     </row>
     <row r="135" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="5" t="n">
+      <c r="A135" s="4" t="n">
         <v>43668.0833333333</v>
       </c>
       <c r="B135" s="2" t="n">
@@ -13343,7 +13342,7 @@
       </c>
     </row>
     <row r="136" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="5" t="n">
+      <c r="A136" s="4" t="n">
         <v>43665.0833333333</v>
       </c>
       <c r="B136" s="2" t="n">
@@ -13354,7 +13353,7 @@
       </c>
     </row>
     <row r="137" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="5" t="n">
+      <c r="A137" s="4" t="n">
         <v>43664.0833333333</v>
       </c>
       <c r="B137" s="2" t="n">
@@ -13365,7 +13364,7 @@
       </c>
     </row>
     <row r="138" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="5" t="n">
+      <c r="A138" s="4" t="n">
         <v>43663.0833333333</v>
       </c>
       <c r="B138" s="2" t="n">
@@ -13376,7 +13375,7 @@
       </c>
     </row>
     <row r="139" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="5" t="n">
+      <c r="A139" s="4" t="n">
         <v>43662.0833333333</v>
       </c>
       <c r="B139" s="2" t="n">
@@ -13387,7 +13386,7 @@
       </c>
     </row>
     <row r="140" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="5" t="n">
+      <c r="A140" s="4" t="n">
         <v>43661.0833333333</v>
       </c>
       <c r="B140" s="2" t="n">
@@ -13398,7 +13397,7 @@
       </c>
     </row>
     <row r="141" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="5" t="n">
+      <c r="A141" s="4" t="n">
         <v>43658.0833333333</v>
       </c>
       <c r="B141" s="2" t="n">
@@ -13409,7 +13408,7 @@
       </c>
     </row>
     <row r="142" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="5" t="n">
+      <c r="A142" s="4" t="n">
         <v>43657.0833333333</v>
       </c>
       <c r="B142" s="2" t="n">
@@ -13420,7 +13419,7 @@
       </c>
     </row>
     <row r="143" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="5" t="n">
+      <c r="A143" s="4" t="n">
         <v>43656.0833333333</v>
       </c>
       <c r="B143" s="2" t="n">
@@ -13431,7 +13430,7 @@
       </c>
     </row>
     <row r="144" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="5" t="n">
+      <c r="A144" s="4" t="n">
         <v>43655.0833333333</v>
       </c>
       <c r="B144" s="2" t="n">
@@ -13442,7 +13441,7 @@
       </c>
     </row>
     <row r="145" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="5" t="n">
+      <c r="A145" s="4" t="n">
         <v>43654.0833333333</v>
       </c>
       <c r="B145" s="2" t="n">
@@ -13453,7 +13452,7 @@
       </c>
     </row>
     <row r="146" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="5" t="n">
+      <c r="A146" s="4" t="n">
         <v>43651.0833333333</v>
       </c>
       <c r="B146" s="2" t="n">
@@ -13464,7 +13463,7 @@
       </c>
     </row>
     <row r="147" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="5" t="n">
+      <c r="A147" s="4" t="n">
         <v>43650.0833333333</v>
       </c>
       <c r="B147" s="2" t="n">
@@ -13475,7 +13474,7 @@
       </c>
     </row>
     <row r="148" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="5" t="n">
+      <c r="A148" s="4" t="n">
         <v>43649.0833333333</v>
       </c>
       <c r="B148" s="2" t="n">
@@ -13486,7 +13485,7 @@
       </c>
     </row>
     <row r="149" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="5" t="n">
+      <c r="A149" s="4" t="n">
         <v>43648.0833333333</v>
       </c>
       <c r="B149" s="2" t="n">
@@ -13497,7 +13496,7 @@
       </c>
     </row>
     <row r="150" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="5" t="n">
+      <c r="A150" s="4" t="n">
         <v>43647.0833333333</v>
       </c>
       <c r="B150" s="2" t="n">
@@ -13508,7 +13507,7 @@
       </c>
     </row>
     <row r="151" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="5" t="n">
+      <c r="A151" s="4" t="n">
         <v>43644.0833333333</v>
       </c>
       <c r="B151" s="2" t="n">
@@ -13519,7 +13518,7 @@
       </c>
     </row>
     <row r="152" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="5" t="n">
+      <c r="A152" s="4" t="n">
         <v>43643.0833333333</v>
       </c>
       <c r="B152" s="2" t="n">
@@ -13530,7 +13529,7 @@
       </c>
     </row>
     <row r="153" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="5" t="n">
+      <c r="A153" s="4" t="n">
         <v>43642.0833333333</v>
       </c>
       <c r="B153" s="2" t="n">
@@ -13541,7 +13540,7 @@
       </c>
     </row>
     <row r="154" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="5" t="n">
+      <c r="A154" s="4" t="n">
         <v>43641.0833333333</v>
       </c>
       <c r="B154" s="2" t="n">
@@ -13552,7 +13551,7 @@
       </c>
     </row>
     <row r="155" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="5" t="n">
+      <c r="A155" s="4" t="n">
         <v>43640.0833333333</v>
       </c>
       <c r="B155" s="2" t="n">
@@ -13563,7 +13562,7 @@
       </c>
     </row>
     <row r="156" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="5" t="n">
+      <c r="A156" s="4" t="n">
         <v>43637.0833333333</v>
       </c>
       <c r="B156" s="2" t="n">
@@ -13574,7 +13573,7 @@
       </c>
     </row>
     <row r="157" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="5" t="n">
+      <c r="A157" s="4" t="n">
         <v>43636.0833333333</v>
       </c>
       <c r="B157" s="2" t="n">
@@ -13585,7 +13584,7 @@
       </c>
     </row>
     <row r="158" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="5" t="n">
+      <c r="A158" s="4" t="n">
         <v>43635.0833333333</v>
       </c>
       <c r="B158" s="2" t="n">
@@ -13596,7 +13595,7 @@
       </c>
     </row>
     <row r="159" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="5" t="n">
+      <c r="A159" s="4" t="n">
         <v>43634.0833333333</v>
       </c>
       <c r="B159" s="2" t="n">
@@ -13607,7 +13606,7 @@
       </c>
     </row>
     <row r="160" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="5" t="n">
+      <c r="A160" s="4" t="n">
         <v>43633.0833333333</v>
       </c>
       <c r="B160" s="2" t="n">
@@ -13618,7 +13617,7 @@
       </c>
     </row>
     <row r="161" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="5" t="n">
+      <c r="A161" s="4" t="n">
         <v>43630.0833333333</v>
       </c>
       <c r="B161" s="2" t="n">
@@ -13629,7 +13628,7 @@
       </c>
     </row>
     <row r="162" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="5" t="n">
+      <c r="A162" s="4" t="n">
         <v>43629.0833333333</v>
       </c>
       <c r="B162" s="2" t="n">
@@ -13640,7 +13639,7 @@
       </c>
     </row>
     <row r="163" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="5" t="n">
+      <c r="A163" s="4" t="n">
         <v>43628.0833333333</v>
       </c>
       <c r="B163" s="2" t="n">
@@ -13651,7 +13650,7 @@
       </c>
     </row>
     <row r="164" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="5" t="n">
+      <c r="A164" s="4" t="n">
         <v>43627.0833333333</v>
       </c>
       <c r="B164" s="2" t="n">
@@ -13662,7 +13661,7 @@
       </c>
     </row>
     <row r="165" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A165" s="5" t="n">
+      <c r="A165" s="4" t="n">
         <v>43626.0833333333</v>
       </c>
       <c r="B165" s="2" t="n">
@@ -13673,7 +13672,7 @@
       </c>
     </row>
     <row r="166" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="5" t="n">
+      <c r="A166" s="4" t="n">
         <v>43623.0833333333</v>
       </c>
       <c r="B166" s="2" t="n">
@@ -13684,7 +13683,7 @@
       </c>
     </row>
     <row r="167" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="5" t="n">
+      <c r="A167" s="4" t="n">
         <v>43622.0833333333</v>
       </c>
       <c r="B167" s="2" t="n">
@@ -13695,7 +13694,7 @@
       </c>
     </row>
     <row r="168" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A168" s="5" t="n">
+      <c r="A168" s="4" t="n">
         <v>43621.0833333333</v>
       </c>
       <c r="B168" s="2" t="n">
@@ -13706,7 +13705,7 @@
       </c>
     </row>
     <row r="169" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="5" t="n">
+      <c r="A169" s="4" t="n">
         <v>43620.0833333333</v>
       </c>
       <c r="B169" s="2" t="n">
@@ -13717,7 +13716,7 @@
       </c>
     </row>
     <row r="170" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="5" t="n">
+      <c r="A170" s="4" t="n">
         <v>43619.0833333333</v>
       </c>
       <c r="B170" s="2" t="n">
@@ -13728,7 +13727,7 @@
       </c>
     </row>
     <row r="171" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A171" s="5" t="n">
+      <c r="A171" s="4" t="n">
         <v>43616.0833333333</v>
       </c>
       <c r="B171" s="2" t="n">
@@ -13739,7 +13738,7 @@
       </c>
     </row>
     <row r="172" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A172" s="5" t="n">
+      <c r="A172" s="4" t="n">
         <v>43615.0833333333</v>
       </c>
       <c r="B172" s="2" t="n">
@@ -13750,7 +13749,7 @@
       </c>
     </row>
     <row r="173" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A173" s="5" t="n">
+      <c r="A173" s="4" t="n">
         <v>43614.0833333333</v>
       </c>
       <c r="B173" s="2" t="n">
@@ -13761,7 +13760,7 @@
       </c>
     </row>
     <row r="174" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A174" s="5" t="n">
+      <c r="A174" s="4" t="n">
         <v>43613.0833333333</v>
       </c>
       <c r="B174" s="2" t="n">
@@ -13772,7 +13771,7 @@
       </c>
     </row>
     <row r="175" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A175" s="5" t="n">
+      <c r="A175" s="4" t="n">
         <v>43609.0833333333</v>
       </c>
       <c r="B175" s="2" t="n">
@@ -13783,7 +13782,7 @@
       </c>
     </row>
     <row r="176" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A176" s="5" t="n">
+      <c r="A176" s="4" t="n">
         <v>43608.0833333333</v>
       </c>
       <c r="B176" s="2" t="n">
@@ -13794,7 +13793,7 @@
       </c>
     </row>
     <row r="177" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="5" t="n">
+      <c r="A177" s="4" t="n">
         <v>43607.0833333333</v>
       </c>
       <c r="B177" s="2" t="n">
@@ -13805,7 +13804,7 @@
       </c>
     </row>
     <row r="178" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="5" t="n">
+      <c r="A178" s="4" t="n">
         <v>43606.0833333333</v>
       </c>
       <c r="B178" s="2" t="n">
@@ -13816,7 +13815,7 @@
       </c>
     </row>
     <row r="179" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="5" t="n">
+      <c r="A179" s="4" t="n">
         <v>43605.0833333333</v>
       </c>
       <c r="B179" s="2" t="n">
@@ -13827,7 +13826,7 @@
       </c>
     </row>
     <row r="180" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="5" t="n">
+      <c r="A180" s="4" t="n">
         <v>43602.0833333333</v>
       </c>
       <c r="B180" s="2" t="n">
@@ -13838,7 +13837,7 @@
       </c>
     </row>
     <row r="181" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A181" s="5" t="n">
+      <c r="A181" s="4" t="n">
         <v>43601.0833333333</v>
       </c>
       <c r="B181" s="2" t="n">
@@ -13849,7 +13848,7 @@
       </c>
     </row>
     <row r="182" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A182" s="5" t="n">
+      <c r="A182" s="4" t="n">
         <v>43600.0833333333</v>
       </c>
       <c r="B182" s="2" t="n">
@@ -13860,7 +13859,7 @@
       </c>
     </row>
     <row r="183" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A183" s="5" t="n">
+      <c r="A183" s="4" t="n">
         <v>43599.0833333333</v>
       </c>
       <c r="B183" s="2" t="n">
@@ -13871,7 +13870,7 @@
       </c>
     </row>
     <row r="184" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A184" s="5" t="n">
+      <c r="A184" s="4" t="n">
         <v>43598.0833333333</v>
       </c>
       <c r="B184" s="2" t="n">
@@ -13882,7 +13881,7 @@
       </c>
     </row>
     <row r="185" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A185" s="5" t="n">
+      <c r="A185" s="4" t="n">
         <v>43595.0833333333</v>
       </c>
       <c r="B185" s="2" t="n">
@@ -13893,7 +13892,7 @@
       </c>
     </row>
     <row r="186" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A186" s="5" t="n">
+      <c r="A186" s="4" t="n">
         <v>43594.0833333333</v>
       </c>
       <c r="B186" s="2" t="n">
@@ -13904,7 +13903,7 @@
       </c>
     </row>
     <row r="187" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A187" s="5" t="n">
+      <c r="A187" s="4" t="n">
         <v>43593.0833333333</v>
       </c>
       <c r="B187" s="2" t="n">
@@ -13915,7 +13914,7 @@
       </c>
     </row>
     <row r="188" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A188" s="5" t="n">
+      <c r="A188" s="4" t="n">
         <v>43592.0833333333</v>
       </c>
       <c r="B188" s="2" t="n">
@@ -13926,7 +13925,7 @@
       </c>
     </row>
     <row r="189" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A189" s="5" t="n">
+      <c r="A189" s="4" t="n">
         <v>43588.0833333333</v>
       </c>
       <c r="B189" s="2" t="n">
@@ -13937,7 +13936,7 @@
       </c>
     </row>
     <row r="190" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A190" s="5" t="n">
+      <c r="A190" s="4" t="n">
         <v>43587.0833333333</v>
       </c>
       <c r="B190" s="2" t="n">
@@ -13948,7 +13947,7 @@
       </c>
     </row>
     <row r="191" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A191" s="5" t="n">
+      <c r="A191" s="4" t="n">
         <v>43586.0833333333</v>
       </c>
       <c r="B191" s="2" t="n">
@@ -13959,7 +13958,7 @@
       </c>
     </row>
     <row r="192" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A192" s="5" t="n">
+      <c r="A192" s="4" t="n">
         <v>43585.0833333333</v>
       </c>
       <c r="B192" s="2" t="n">
@@ -13970,7 +13969,7 @@
       </c>
     </row>
     <row r="193" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A193" s="5" t="n">
+      <c r="A193" s="4" t="n">
         <v>43584.0833333333</v>
       </c>
       <c r="B193" s="2" t="n">
@@ -13981,7 +13980,7 @@
       </c>
     </row>
     <row r="194" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A194" s="5" t="n">
+      <c r="A194" s="4" t="n">
         <v>43581.0833333333</v>
       </c>
       <c r="B194" s="2" t="n">
@@ -13992,7 +13991,7 @@
       </c>
     </row>
     <row r="195" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A195" s="5" t="n">
+      <c r="A195" s="4" t="n">
         <v>43580.0833333333</v>
       </c>
       <c r="B195" s="2" t="n">
@@ -14003,7 +14002,7 @@
       </c>
     </row>
     <row r="196" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A196" s="5" t="n">
+      <c r="A196" s="4" t="n">
         <v>43579.0833333333</v>
       </c>
       <c r="B196" s="2" t="n">
@@ -14014,7 +14013,7 @@
       </c>
     </row>
     <row r="197" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A197" s="5" t="n">
+      <c r="A197" s="4" t="n">
         <v>43578.0833333333</v>
       </c>
       <c r="B197" s="2" t="n">
@@ -14025,7 +14024,7 @@
       </c>
     </row>
     <row r="198" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A198" s="5" t="n">
+      <c r="A198" s="4" t="n">
         <v>43573.0833333333</v>
       </c>
       <c r="B198" s="2" t="n">
@@ -14036,7 +14035,7 @@
       </c>
     </row>
     <row r="199" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A199" s="5" t="n">
+      <c r="A199" s="4" t="n">
         <v>43572.0833333333</v>
       </c>
       <c r="B199" s="2" t="n">
@@ -14047,7 +14046,7 @@
       </c>
     </row>
     <row r="200" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A200" s="5" t="n">
+      <c r="A200" s="4" t="n">
         <v>43571.0833333333</v>
       </c>
       <c r="B200" s="2" t="n">
@@ -14058,7 +14057,7 @@
       </c>
     </row>
     <row r="201" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A201" s="5" t="n">
+      <c r="A201" s="4" t="n">
         <v>43570.0833333333</v>
       </c>
       <c r="B201" s="2" t="n">
@@ -14069,7 +14068,7 @@
       </c>
     </row>
     <row r="202" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A202" s="5" t="n">
+      <c r="A202" s="4" t="n">
         <v>43567.0833333333</v>
       </c>
       <c r="B202" s="2" t="n">
@@ -14080,7 +14079,7 @@
       </c>
     </row>
     <row r="203" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A203" s="5" t="n">
+      <c r="A203" s="4" t="n">
         <v>43566.0833333333</v>
       </c>
       <c r="B203" s="2" t="n">
@@ -14091,7 +14090,7 @@
       </c>
     </row>
     <row r="204" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A204" s="5" t="n">
+      <c r="A204" s="4" t="n">
         <v>43565.0833333333</v>
       </c>
       <c r="B204" s="2" t="n">
@@ -14102,7 +14101,7 @@
       </c>
     </row>
     <row r="205" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A205" s="5" t="n">
+      <c r="A205" s="4" t="n">
         <v>43564.0833333333</v>
       </c>
       <c r="B205" s="2" t="n">
@@ -14113,7 +14112,7 @@
       </c>
     </row>
     <row r="206" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A206" s="5" t="n">
+      <c r="A206" s="4" t="n">
         <v>43563.0833333333</v>
       </c>
       <c r="B206" s="2" t="n">
@@ -14124,7 +14123,7 @@
       </c>
     </row>
     <row r="207" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A207" s="5" t="n">
+      <c r="A207" s="4" t="n">
         <v>43560.0833333333</v>
       </c>
       <c r="B207" s="2" t="n">
@@ -14135,7 +14134,7 @@
       </c>
     </row>
     <row r="208" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A208" s="5" t="n">
+      <c r="A208" s="4" t="n">
         <v>43559.0833333333</v>
       </c>
       <c r="B208" s="2" t="n">
@@ -14146,7 +14145,7 @@
       </c>
     </row>
     <row r="209" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A209" s="5" t="n">
+      <c r="A209" s="4" t="n">
         <v>43558.0833333333</v>
       </c>
       <c r="B209" s="2" t="n">
@@ -14157,7 +14156,7 @@
       </c>
     </row>
     <row r="210" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A210" s="5" t="n">
+      <c r="A210" s="4" t="n">
         <v>43557.0833333333</v>
       </c>
       <c r="B210" s="2" t="n">
@@ -14168,7 +14167,7 @@
       </c>
     </row>
     <row r="211" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A211" s="5" t="n">
+      <c r="A211" s="4" t="n">
         <v>43556.0833333333</v>
       </c>
       <c r="B211" s="2" t="n">
@@ -14179,7 +14178,7 @@
       </c>
     </row>
     <row r="212" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A212" s="5" t="n">
+      <c r="A212" s="4" t="n">
         <v>43553.0416666667</v>
       </c>
       <c r="B212" s="2" t="n">
@@ -14190,7 +14189,7 @@
       </c>
     </row>
     <row r="213" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A213" s="5" t="n">
+      <c r="A213" s="4" t="n">
         <v>43552.0416666667</v>
       </c>
       <c r="B213" s="2" t="n">
@@ -14201,7 +14200,7 @@
       </c>
     </row>
     <row r="214" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A214" s="5" t="n">
+      <c r="A214" s="4" t="n">
         <v>43551.0416666667</v>
       </c>
       <c r="B214" s="2" t="n">
@@ -14212,7 +14211,7 @@
       </c>
     </row>
     <row r="215" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A215" s="5" t="n">
+      <c r="A215" s="4" t="n">
         <v>43550.0416666667</v>
       </c>
       <c r="B215" s="2" t="n">
@@ -14223,7 +14222,7 @@
       </c>
     </row>
     <row r="216" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A216" s="5" t="n">
+      <c r="A216" s="4" t="n">
         <v>43549.0416666667</v>
       </c>
       <c r="B216" s="2" t="n">
@@ -14234,7 +14233,7 @@
       </c>
     </row>
     <row r="217" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A217" s="5" t="n">
+      <c r="A217" s="4" t="n">
         <v>43546.0416666667</v>
       </c>
       <c r="B217" s="2" t="n">
@@ -14245,7 +14244,7 @@
       </c>
     </row>
     <row r="218" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A218" s="5" t="n">
+      <c r="A218" s="4" t="n">
         <v>43545.0416666667</v>
       </c>
       <c r="B218" s="2" t="n">
@@ -14256,7 +14255,7 @@
       </c>
     </row>
     <row r="219" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A219" s="5" t="n">
+      <c r="A219" s="4" t="n">
         <v>43544.0416666667</v>
       </c>
       <c r="B219" s="2" t="n">
@@ -14267,7 +14266,7 @@
       </c>
     </row>
     <row r="220" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A220" s="5" t="n">
+      <c r="A220" s="4" t="n">
         <v>43543.0416666667</v>
       </c>
       <c r="B220" s="2" t="n">
@@ -14278,7 +14277,7 @@
       </c>
     </row>
     <row r="221" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A221" s="5" t="n">
+      <c r="A221" s="4" t="n">
         <v>43542.0416666667</v>
       </c>
       <c r="B221" s="2" t="n">
@@ -14289,7 +14288,7 @@
       </c>
     </row>
     <row r="222" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A222" s="5" t="n">
+      <c r="A222" s="4" t="n">
         <v>43539.0416666667</v>
       </c>
       <c r="B222" s="2" t="n">
@@ -14300,7 +14299,7 @@
       </c>
     </row>
     <row r="223" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A223" s="5" t="n">
+      <c r="A223" s="4" t="n">
         <v>43538.0416666667</v>
       </c>
       <c r="B223" s="2" t="n">
@@ -14311,7 +14310,7 @@
       </c>
     </row>
     <row r="224" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A224" s="5" t="n">
+      <c r="A224" s="4" t="n">
         <v>43537.0416666667</v>
       </c>
       <c r="B224" s="2" t="n">
@@ -14322,7 +14321,7 @@
       </c>
     </row>
     <row r="225" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A225" s="5" t="n">
+      <c r="A225" s="4" t="n">
         <v>43536.0416666667</v>
       </c>
       <c r="B225" s="2" t="n">
@@ -14333,7 +14332,7 @@
       </c>
     </row>
     <row r="226" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A226" s="5" t="n">
+      <c r="A226" s="4" t="n">
         <v>43535.0416666667</v>
       </c>
       <c r="B226" s="2" t="n">
@@ -14344,7 +14343,7 @@
       </c>
     </row>
     <row r="227" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A227" s="5" t="n">
+      <c r="A227" s="4" t="n">
         <v>43532.0416666667</v>
       </c>
       <c r="B227" s="2" t="n">
@@ -14355,7 +14354,7 @@
       </c>
     </row>
     <row r="228" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A228" s="5" t="n">
+      <c r="A228" s="4" t="n">
         <v>43531.0416666667</v>
       </c>
       <c r="B228" s="2" t="n">
@@ -14366,7 +14365,7 @@
       </c>
     </row>
     <row r="229" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A229" s="5" t="n">
+      <c r="A229" s="4" t="n">
         <v>43530.0416666667</v>
       </c>
       <c r="B229" s="2" t="n">
@@ -14377,7 +14376,7 @@
       </c>
     </row>
     <row r="230" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A230" s="5" t="n">
+      <c r="A230" s="4" t="n">
         <v>43529.0416666667</v>
       </c>
       <c r="B230" s="2" t="n">
@@ -14388,7 +14387,7 @@
       </c>
     </row>
     <row r="231" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A231" s="5" t="n">
+      <c r="A231" s="4" t="n">
         <v>43528.0416666667</v>
       </c>
       <c r="B231" s="2" t="n">
@@ -14399,7 +14398,7 @@
       </c>
     </row>
     <row r="232" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A232" s="5" t="n">
+      <c r="A232" s="4" t="n">
         <v>43525.0416666667</v>
       </c>
       <c r="B232" s="2" t="n">
@@ -14410,7 +14409,7 @@
       </c>
     </row>
     <row r="233" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A233" s="5" t="n">
+      <c r="A233" s="4" t="n">
         <v>43524.0416666667</v>
       </c>
       <c r="B233" s="2" t="n">
@@ -14421,7 +14420,7 @@
       </c>
     </row>
     <row r="234" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A234" s="5" t="n">
+      <c r="A234" s="4" t="n">
         <v>43523.0416666667</v>
       </c>
       <c r="B234" s="2" t="n">
@@ -14432,7 +14431,7 @@
       </c>
     </row>
     <row r="235" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A235" s="5" t="n">
+      <c r="A235" s="4" t="n">
         <v>43522.0416666667</v>
       </c>
       <c r="B235" s="2" t="n">
@@ -14443,7 +14442,7 @@
       </c>
     </row>
     <row r="236" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A236" s="5" t="n">
+      <c r="A236" s="4" t="n">
         <v>43521.0416666667</v>
       </c>
       <c r="B236" s="2" t="n">
@@ -14454,7 +14453,7 @@
       </c>
     </row>
     <row r="237" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A237" s="5" t="n">
+      <c r="A237" s="4" t="n">
         <v>43518.0416666667</v>
       </c>
       <c r="B237" s="2" t="n">
@@ -14465,7 +14464,7 @@
       </c>
     </row>
     <row r="238" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A238" s="5" t="n">
+      <c r="A238" s="4" t="n">
         <v>43517.0416666667</v>
       </c>
       <c r="B238" s="2" t="n">
@@ -14476,7 +14475,7 @@
       </c>
     </row>
     <row r="239" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A239" s="5" t="n">
+      <c r="A239" s="4" t="n">
         <v>43516.0416666667</v>
       </c>
       <c r="B239" s="2" t="n">
@@ -14487,7 +14486,7 @@
       </c>
     </row>
     <row r="240" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A240" s="5" t="n">
+      <c r="A240" s="4" t="n">
         <v>43515.0416666667</v>
       </c>
       <c r="B240" s="2" t="n">
@@ -14498,7 +14497,7 @@
       </c>
     </row>
     <row r="241" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A241" s="5" t="n">
+      <c r="A241" s="4" t="n">
         <v>43514.0416666667</v>
       </c>
       <c r="B241" s="2" t="n">
@@ -14509,7 +14508,7 @@
       </c>
     </row>
     <row r="242" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A242" s="5" t="n">
+      <c r="A242" s="4" t="n">
         <v>43511.0416666667</v>
       </c>
       <c r="B242" s="2" t="n">
@@ -14520,7 +14519,7 @@
       </c>
     </row>
     <row r="243" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A243" s="5" t="n">
+      <c r="A243" s="4" t="n">
         <v>43510.0416666667</v>
       </c>
       <c r="B243" s="2" t="n">
@@ -14531,7 +14530,7 @@
       </c>
     </row>
     <row r="244" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A244" s="5" t="n">
+      <c r="A244" s="4" t="n">
         <v>43509.0416666667</v>
       </c>
       <c r="B244" s="2" t="n">
@@ -14542,7 +14541,7 @@
       </c>
     </row>
     <row r="245" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A245" s="5" t="n">
+      <c r="A245" s="4" t="n">
         <v>43508.0416666667</v>
       </c>
       <c r="B245" s="2" t="n">
@@ -14553,7 +14552,7 @@
       </c>
     </row>
     <row r="246" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A246" s="5" t="n">
+      <c r="A246" s="4" t="n">
         <v>43507.0416666667</v>
       </c>
       <c r="B246" s="2" t="n">
@@ -14564,7 +14563,7 @@
       </c>
     </row>
     <row r="247" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A247" s="5" t="n">
+      <c r="A247" s="4" t="n">
         <v>43504.0416666667</v>
       </c>
       <c r="B247" s="2" t="n">
@@ -14575,7 +14574,7 @@
       </c>
     </row>
     <row r="248" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A248" s="5" t="n">
+      <c r="A248" s="4" t="n">
         <v>43503.0416666667</v>
       </c>
       <c r="B248" s="2" t="n">
@@ -14586,7 +14585,7 @@
       </c>
     </row>
     <row r="249" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A249" s="5" t="n">
+      <c r="A249" s="4" t="n">
         <v>43502.0416666667</v>
       </c>
       <c r="B249" s="2" t="n">
@@ -14597,7 +14596,7 @@
       </c>
     </row>
     <row r="250" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A250" s="5" t="n">
+      <c r="A250" s="4" t="n">
         <v>43501.0416666667</v>
       </c>
       <c r="B250" s="2" t="n">
@@ -14608,7 +14607,7 @@
       </c>
     </row>
     <row r="251" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A251" s="5" t="n">
+      <c r="A251" s="4" t="n">
         <v>43500.0416666667</v>
       </c>
       <c r="B251" s="2" t="n">
@@ -14619,7 +14618,7 @@
       </c>
     </row>
     <row r="252" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A252" s="5" t="n">
+      <c r="A252" s="4" t="n">
         <v>43497.0416666667</v>
       </c>
       <c r="B252" s="2" t="n">
@@ -14630,7 +14629,7 @@
       </c>
     </row>
     <row r="253" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A253" s="5" t="n">
+      <c r="A253" s="4" t="n">
         <v>43496.0416666667</v>
       </c>
       <c r="B253" s="2" t="n">
@@ -14641,7 +14640,7 @@
       </c>
     </row>
     <row r="254" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A254" s="5" t="n">
+      <c r="A254" s="4" t="n">
         <v>43495.0416666667</v>
       </c>
       <c r="B254" s="2" t="n">
@@ -14651,8 +14650,8 @@
         <v>47.74</v>
       </c>
     </row>
-    <row r="255" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A255" s="5" t="n">
+    <row r="255" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A255" s="4" t="n">
         <v>43494.0416666667</v>
       </c>
       <c r="B255" s="2" t="n">
@@ -14681,8 +14680,8 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L28" activeCellId="0" sqref="L28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L28" activeCellId="1" sqref="A:A L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14709,7 +14708,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M28" activeCellId="0" sqref="M28"/>
+      <selection pane="topLeft" activeCell="M28" activeCellId="1" sqref="A:A M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
fixed year lenght in case one year ago was easter or sth
</commit_message>
<xml_diff>
--- a/code/scripts/RACF_Fuel_factsheet_template.xlsx
+++ b/code/scripts/RACF_Fuel_factsheet_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="master" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,7 +16,7 @@
     <sheet name="oil.chart" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" name="pump_prices" vbProcedure="false">'pump.chart.data'!$A$1:$C$254</definedName>
+    <definedName function="false" hidden="false" name="pump_prices" vbProcedure="false">'pump.chart.data'!$A$1:$C$252</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -863,11 +863,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="34724557"/>
-        <c:axId val="25069989"/>
+        <c:axId val="75957915"/>
+        <c:axId val="64889910"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="34724557"/>
+        <c:axId val="75957915"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -895,14 +895,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="25069989"/>
+        <c:crossAx val="64889910"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="25069989"/>
+        <c:axId val="64889910"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -939,7 +939,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="34724557"/>
+        <c:crossAx val="75957915"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -980,7 +980,7 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
@@ -1048,778 +1048,769 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'pump.chart.data'!$A$2:$A$258</c:f>
+              <c:f>'pump.chart.data'!$A$2:$A$255</c:f>
               <c:strCache>
-                <c:ptCount val="257"/>
+                <c:ptCount val="254"/>
                 <c:pt idx="0">
-                  <c:v>29-01-2020</c:v>
+                  <c:v>29/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>28-01-2020</c:v>
+                  <c:v>28/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>27-01-2020</c:v>
+                  <c:v>27/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24-01-2020</c:v>
+                  <c:v>24/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23-01-2020</c:v>
+                  <c:v>23/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>22-01-2020</c:v>
+                  <c:v>22/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21-01-2020</c:v>
+                  <c:v>21/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>20-01-2020</c:v>
+                  <c:v>20/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>17-01-2020</c:v>
+                  <c:v>17/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>16-01-2020</c:v>
+                  <c:v>16/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>15-01-2020</c:v>
+                  <c:v>15/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>14-01-2020</c:v>
+                  <c:v>14/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>13-01-2020</c:v>
+                  <c:v>13/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>10-01-2020</c:v>
+                  <c:v>10/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>09-01-2020</c:v>
+                  <c:v>09/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>08-01-2020</c:v>
+                  <c:v>08/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>07-01-2020</c:v>
+                  <c:v>07/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>06-01-2020</c:v>
+                  <c:v>06/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>03-01-2020</c:v>
+                  <c:v>03/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>02-01-2020</c:v>
+                  <c:v>02/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>31-12-2019</c:v>
+                  <c:v>31/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>30-12-2019</c:v>
+                  <c:v>30/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>27-12-2019</c:v>
+                  <c:v>27/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>24-12-2019</c:v>
+                  <c:v>24/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>23-12-2019</c:v>
+                  <c:v>23/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>20-12-2019</c:v>
+                  <c:v>20/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>19-12-2019</c:v>
+                  <c:v>19/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>18-12-2019</c:v>
+                  <c:v>18/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>17-12-2019</c:v>
+                  <c:v>17/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>16-12-2019</c:v>
+                  <c:v>16/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>13-12-2019</c:v>
+                  <c:v>13/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>12-12-2019</c:v>
+                  <c:v>12/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>11-12-2019</c:v>
+                  <c:v>11/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>10-12-2019</c:v>
+                  <c:v>10/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>09-12-2019</c:v>
+                  <c:v>09/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>06-12-2019</c:v>
+                  <c:v>06/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>05-12-2019</c:v>
+                  <c:v>05/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>04-12-2019</c:v>
+                  <c:v>04/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>03-12-2019</c:v>
+                  <c:v>03/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>02-12-2019</c:v>
+                  <c:v>02/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>29-11-2019</c:v>
+                  <c:v>29/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>28-11-2019</c:v>
+                  <c:v>28/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>27-11-2019</c:v>
+                  <c:v>27/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>26-11-2019</c:v>
+                  <c:v>26/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>25-11-2019</c:v>
+                  <c:v>25/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>22-11-2019</c:v>
+                  <c:v>22/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>21-11-2019</c:v>
+                  <c:v>21/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>20-11-2019</c:v>
+                  <c:v>20/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>19-11-2019</c:v>
+                  <c:v>19/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>18-11-2019</c:v>
+                  <c:v>18/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>15-11-2019</c:v>
+                  <c:v>15/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>14-11-2019</c:v>
+                  <c:v>14/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>13-11-2019</c:v>
+                  <c:v>13/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>12-11-2019</c:v>
+                  <c:v>12/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>11-11-2019</c:v>
+                  <c:v>11/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>08-11-2019</c:v>
+                  <c:v>08/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>07-11-2019</c:v>
+                  <c:v>07/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>06-11-2019</c:v>
+                  <c:v>06/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>05-11-2019</c:v>
+                  <c:v>05/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>04-11-2019</c:v>
+                  <c:v>04/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>01-11-2019</c:v>
+                  <c:v>01/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>31-10-2019</c:v>
+                  <c:v>31/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>30-10-2019</c:v>
+                  <c:v>30/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>29-10-2019</c:v>
+                  <c:v>29/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>28-10-2019</c:v>
+                  <c:v>28/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>25-10-2019</c:v>
+                  <c:v>25/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>24-10-2019</c:v>
+                  <c:v>24/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>23-10-2019</c:v>
+                  <c:v>23/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>22-10-2019</c:v>
+                  <c:v>22/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>21-10-2019</c:v>
+                  <c:v>21/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>18-10-2019</c:v>
+                  <c:v>18/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>17-10-2019</c:v>
+                  <c:v>17/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>16-10-2019</c:v>
+                  <c:v>16/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>15-10-2019</c:v>
+                  <c:v>15/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>14-10-2019</c:v>
+                  <c:v>14/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>11-10-2019</c:v>
+                  <c:v>11/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>10-10-2019</c:v>
+                  <c:v>10/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>09-10-2019</c:v>
+                  <c:v>09/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>08-10-2019</c:v>
+                  <c:v>08/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>07-10-2019</c:v>
+                  <c:v>07/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>04-10-2019</c:v>
+                  <c:v>04/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>03-10-2019</c:v>
+                  <c:v>03/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>02-10-2019</c:v>
+                  <c:v>02/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>01-10-2019</c:v>
+                  <c:v>01/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>30-09-2019</c:v>
+                  <c:v>30/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>27-09-2019</c:v>
+                  <c:v>27/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>26-09-2019</c:v>
+                  <c:v>26/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>25-09-2019</c:v>
+                  <c:v>25/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>24-09-2019</c:v>
+                  <c:v>24/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>23-09-2019</c:v>
+                  <c:v>23/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>20-09-2019</c:v>
+                  <c:v>20/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>19-09-2019</c:v>
+                  <c:v>19/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>18-09-2019</c:v>
+                  <c:v>18/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>17-09-2019</c:v>
+                  <c:v>17/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>16-09-2019</c:v>
+                  <c:v>16/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>13-09-2019</c:v>
+                  <c:v>13/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>12-09-2019</c:v>
+                  <c:v>12/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>11-09-2019</c:v>
+                  <c:v>11/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>10-09-2019</c:v>
+                  <c:v>10/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>09-09-2019</c:v>
+                  <c:v>09/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>06-09-2019</c:v>
+                  <c:v>06/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>05-09-2019</c:v>
+                  <c:v>05/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>04-09-2019</c:v>
+                  <c:v>04/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>03-09-2019</c:v>
+                  <c:v>03/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>02-09-2019</c:v>
+                  <c:v>02/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>30-08-2019</c:v>
+                  <c:v>30/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>29-08-2019</c:v>
+                  <c:v>29/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>28-08-2019</c:v>
+                  <c:v>28/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>27-08-2019</c:v>
+                  <c:v>27/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>23-08-2019</c:v>
+                  <c:v>23/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>22-08-2019</c:v>
+                  <c:v>22/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>21-08-2019</c:v>
+                  <c:v>21/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>20-08-2019</c:v>
+                  <c:v>20/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>19-08-2019</c:v>
+                  <c:v>19/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>16-08-2019</c:v>
+                  <c:v>16/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>15-08-2019</c:v>
+                  <c:v>15/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>14-08-2019</c:v>
+                  <c:v>14/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>13-08-2019</c:v>
+                  <c:v>13/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>12-08-2019</c:v>
+                  <c:v>12/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>09-08-2019</c:v>
+                  <c:v>09/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>08-08-2019</c:v>
+                  <c:v>08/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>07-08-2019</c:v>
+                  <c:v>07/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>06-08-2019</c:v>
+                  <c:v>06/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>05-08-2019</c:v>
+                  <c:v>05/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>02-08-2019</c:v>
+                  <c:v>02/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>01-08-2019</c:v>
+                  <c:v>01/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>31-07-2019</c:v>
+                  <c:v>31/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>30-07-2019</c:v>
+                  <c:v>30/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>29-07-2019</c:v>
+                  <c:v>29/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>26-07-2019</c:v>
+                  <c:v>26/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>25-07-2019</c:v>
+                  <c:v>25/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>24-07-2019</c:v>
+                  <c:v>24/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>23-07-2019</c:v>
+                  <c:v>23/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>22-07-2019</c:v>
+                  <c:v>22/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>19-07-2019</c:v>
+                  <c:v>19/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>18-07-2019</c:v>
+                  <c:v>18/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="136">
-                  <c:v>17-07-2019</c:v>
+                  <c:v>17/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="137">
-                  <c:v>16-07-2019</c:v>
+                  <c:v>16/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="138">
-                  <c:v>15-07-2019</c:v>
+                  <c:v>15/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="139">
-                  <c:v>12-07-2019</c:v>
+                  <c:v>12/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>11-07-2019</c:v>
+                  <c:v>11/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="141">
-                  <c:v>10-07-2019</c:v>
+                  <c:v>10/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="142">
-                  <c:v>09-07-2019</c:v>
+                  <c:v>09/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>08-07-2019</c:v>
+                  <c:v>08/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="144">
-                  <c:v>05-07-2019</c:v>
+                  <c:v>05/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="145">
-                  <c:v>04-07-2019</c:v>
+                  <c:v>04/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="146">
-                  <c:v>03-07-2019</c:v>
+                  <c:v>03/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="147">
-                  <c:v>02-07-2019</c:v>
+                  <c:v>02/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="148">
-                  <c:v>01-07-2019</c:v>
+                  <c:v>01/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="149">
-                  <c:v>28-06-2019</c:v>
+                  <c:v>28/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="150">
-                  <c:v>27-06-2019</c:v>
+                  <c:v>27/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="151">
-                  <c:v>26-06-2019</c:v>
+                  <c:v>26/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="152">
-                  <c:v>25-06-2019</c:v>
+                  <c:v>25/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="153">
-                  <c:v>24-06-2019</c:v>
+                  <c:v>24/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="154">
-                  <c:v>21-06-2019</c:v>
+                  <c:v>21/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="155">
-                  <c:v>20-06-2019</c:v>
+                  <c:v>20/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="156">
-                  <c:v>19-06-2019</c:v>
+                  <c:v>19/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="157">
-                  <c:v>18-06-2019</c:v>
+                  <c:v>18/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="158">
-                  <c:v>17-06-2019</c:v>
+                  <c:v>17/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="159">
-                  <c:v>14-06-2019</c:v>
+                  <c:v>14/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="160">
-                  <c:v>13-06-2019</c:v>
+                  <c:v>13/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="161">
-                  <c:v>12-06-2019</c:v>
+                  <c:v>12/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="162">
-                  <c:v>11-06-2019</c:v>
+                  <c:v>11/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="163">
-                  <c:v>10-06-2019</c:v>
+                  <c:v>10/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="164">
-                  <c:v>07-06-2019</c:v>
+                  <c:v>07/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="165">
-                  <c:v>06-06-2019</c:v>
+                  <c:v>06/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="166">
-                  <c:v>05-06-2019</c:v>
+                  <c:v>05/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="167">
-                  <c:v>04-06-2019</c:v>
+                  <c:v>04/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="168">
-                  <c:v>03-06-2019</c:v>
+                  <c:v>03/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="169">
-                  <c:v>31-05-2019</c:v>
+                  <c:v>31/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="170">
-                  <c:v>30-05-2019</c:v>
+                  <c:v>30/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="171">
-                  <c:v>29-05-2019</c:v>
+                  <c:v>29/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="172">
-                  <c:v>28-05-2019</c:v>
+                  <c:v>28/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="173">
-                  <c:v>24-05-2019</c:v>
+                  <c:v>24/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="174">
-                  <c:v>23-05-2019</c:v>
+                  <c:v>23/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="175">
-                  <c:v>22-05-2019</c:v>
+                  <c:v>22/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="176">
-                  <c:v>21-05-2019</c:v>
+                  <c:v>21/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="177">
-                  <c:v>20-05-2019</c:v>
+                  <c:v>20/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="178">
-                  <c:v>17-05-2019</c:v>
+                  <c:v>17/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="179">
-                  <c:v>16-05-2019</c:v>
+                  <c:v>16/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="180">
-                  <c:v>15-05-2019</c:v>
+                  <c:v>15/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="181">
-                  <c:v>14-05-2019</c:v>
+                  <c:v>14/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="182">
-                  <c:v>13-05-2019</c:v>
+                  <c:v>13/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="183">
-                  <c:v>10-05-2019</c:v>
+                  <c:v>10/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="184">
-                  <c:v>09-05-2019</c:v>
+                  <c:v>09/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="185">
-                  <c:v>08-05-2019</c:v>
+                  <c:v>08/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="186">
-                  <c:v>07-05-2019</c:v>
+                  <c:v>07/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="187">
-                  <c:v>03-05-2019</c:v>
+                  <c:v>03/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="188">
-                  <c:v>02-05-2019</c:v>
+                  <c:v>02/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="189">
-                  <c:v>01-05-2019</c:v>
+                  <c:v>01/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="190">
-                  <c:v>30-04-2019</c:v>
+                  <c:v>30/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="191">
-                  <c:v>29-04-2019</c:v>
+                  <c:v>29/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="192">
-                  <c:v>26-04-2019</c:v>
+                  <c:v>26/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="193">
-                  <c:v>25-04-2019</c:v>
+                  <c:v>25/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="194">
-                  <c:v>24-04-2019</c:v>
+                  <c:v>24/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="195">
-                  <c:v>23-04-2019</c:v>
+                  <c:v>23/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="196">
-                  <c:v>18-04-2019</c:v>
+                  <c:v>18/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="197">
-                  <c:v>17-04-2019</c:v>
+                  <c:v>17/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="198">
-                  <c:v>16-04-2019</c:v>
+                  <c:v>16/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="199">
-                  <c:v>15-04-2019</c:v>
+                  <c:v>15/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="200">
-                  <c:v>12-04-2019</c:v>
+                  <c:v>12/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="201">
-                  <c:v>11-04-2019</c:v>
+                  <c:v>11/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="202">
-                  <c:v>10-04-2019</c:v>
+                  <c:v>10/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="203">
-                  <c:v>09-04-2019</c:v>
+                  <c:v>09/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="204">
-                  <c:v>08-04-2019</c:v>
+                  <c:v>08/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="205">
-                  <c:v>05-04-2019</c:v>
+                  <c:v>05/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="206">
-                  <c:v>04-04-2019</c:v>
+                  <c:v>04/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="207">
-                  <c:v>03-04-2019</c:v>
+                  <c:v>03/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="208">
-                  <c:v>02-04-2019</c:v>
+                  <c:v>02/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="209">
-                  <c:v>01-04-2019</c:v>
+                  <c:v>01/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="210">
-                  <c:v>29-03-2019</c:v>
+                  <c:v>29/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="211">
-                  <c:v>28-03-2019</c:v>
+                  <c:v>28/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="212">
-                  <c:v>27-03-2019</c:v>
+                  <c:v>27/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="213">
-                  <c:v>26-03-2019</c:v>
+                  <c:v>26/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="214">
-                  <c:v>25-03-2019</c:v>
+                  <c:v>25/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="215">
-                  <c:v>22-03-2019</c:v>
+                  <c:v>22/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="216">
-                  <c:v>21-03-2019</c:v>
+                  <c:v>21/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="217">
-                  <c:v>20-03-2019</c:v>
+                  <c:v>20/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="218">
-                  <c:v>19-03-2019</c:v>
+                  <c:v>19/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="219">
-                  <c:v>18-03-2019</c:v>
+                  <c:v>18/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="220">
-                  <c:v>15-03-2019</c:v>
+                  <c:v>15/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="221">
-                  <c:v>14-03-2019</c:v>
+                  <c:v>14/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="222">
-                  <c:v>13-03-2019</c:v>
+                  <c:v>13/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="223">
-                  <c:v>12-03-2019</c:v>
+                  <c:v>12/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="224">
-                  <c:v>11-03-2019</c:v>
+                  <c:v>11/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="225">
-                  <c:v>08-03-2019</c:v>
+                  <c:v>08/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="226">
-                  <c:v>07-03-2019</c:v>
+                  <c:v>07/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="227">
-                  <c:v>06-03-2019</c:v>
+                  <c:v>06/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="228">
-                  <c:v>05-03-2019</c:v>
+                  <c:v>05/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="229">
-                  <c:v>04-03-2019</c:v>
+                  <c:v>04/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="230">
-                  <c:v>01-03-2019</c:v>
+                  <c:v>01/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="231">
-                  <c:v>28-02-2019</c:v>
+                  <c:v>28/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="232">
-                  <c:v>27-02-2019</c:v>
+                  <c:v>27/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="233">
-                  <c:v>26-02-2019</c:v>
+                  <c:v>26/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="234">
-                  <c:v>25-02-2019</c:v>
+                  <c:v>25/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="235">
-                  <c:v>22-02-2019</c:v>
+                  <c:v>22/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="236">
-                  <c:v>21-02-2019</c:v>
+                  <c:v>21/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="237">
-                  <c:v>20-02-2019</c:v>
+                  <c:v>20/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="238">
-                  <c:v>19-02-2019</c:v>
+                  <c:v>19/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="239">
-                  <c:v>18-02-2019</c:v>
+                  <c:v>18/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="240">
-                  <c:v>15-02-2019</c:v>
+                  <c:v>15/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="241">
-                  <c:v>14-02-2019</c:v>
+                  <c:v>14/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="242">
-                  <c:v>13-02-2019</c:v>
+                  <c:v>13/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="243">
-                  <c:v>12-02-2019</c:v>
+                  <c:v>12/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="244">
-                  <c:v>11-02-2019</c:v>
+                  <c:v>11/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="245">
-                  <c:v>08-02-2019</c:v>
+                  <c:v>08/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="246">
-                  <c:v>07-02-2019</c:v>
+                  <c:v>07/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="247">
-                  <c:v>06-02-2019</c:v>
+                  <c:v>06/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="248">
-                  <c:v>05-02-2019</c:v>
+                  <c:v>05/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="249">
-                  <c:v>04-02-2019</c:v>
+                  <c:v>04/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="250">
-                  <c:v>01-02-2019</c:v>
+                  <c:v>01/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="251">
-                  <c:v>31-01-2019</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="252">
-                  <c:v>30-01-2019</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="253">
-                  <c:v>29-01-2019</c:v>
-                </c:pt>
-                <c:pt idx="254">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="255">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="256">
                   <c:v/>
                 </c:pt>
               </c:strCache>
@@ -1827,10 +1818,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'pump.chart.data'!$B$2:$B$258</c:f>
+              <c:f>'pump.chart.data'!$B$2:$B$255</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="257"/>
+                <c:ptCount val="254"/>
                 <c:pt idx="0">
                   <c:v>128.05</c:v>
                 </c:pt>
@@ -2583,24 +2574,6 @@
                 </c:pt>
                 <c:pt idx="250">
                   <c:v>119.6</c:v>
-                </c:pt>
-                <c:pt idx="251">
-                  <c:v>119.65</c:v>
-                </c:pt>
-                <c:pt idx="252">
-                  <c:v>119.65</c:v>
-                </c:pt>
-                <c:pt idx="253">
-                  <c:v>119.82</c:v>
-                </c:pt>
-                <c:pt idx="254">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="255">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="256">
-                  <c:v/>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2659,778 +2632,769 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'pump.chart.data'!$A$2:$A$258</c:f>
+              <c:f>'pump.chart.data'!$A$2:$A$255</c:f>
               <c:strCache>
-                <c:ptCount val="257"/>
+                <c:ptCount val="254"/>
                 <c:pt idx="0">
-                  <c:v>29-01-2020</c:v>
+                  <c:v>29/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>28-01-2020</c:v>
+                  <c:v>28/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>27-01-2020</c:v>
+                  <c:v>27/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24-01-2020</c:v>
+                  <c:v>24/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23-01-2020</c:v>
+                  <c:v>23/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>22-01-2020</c:v>
+                  <c:v>22/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21-01-2020</c:v>
+                  <c:v>21/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>20-01-2020</c:v>
+                  <c:v>20/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>17-01-2020</c:v>
+                  <c:v>17/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>16-01-2020</c:v>
+                  <c:v>16/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>15-01-2020</c:v>
+                  <c:v>15/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>14-01-2020</c:v>
+                  <c:v>14/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>13-01-2020</c:v>
+                  <c:v>13/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>10-01-2020</c:v>
+                  <c:v>10/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>09-01-2020</c:v>
+                  <c:v>09/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>08-01-2020</c:v>
+                  <c:v>08/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>07-01-2020</c:v>
+                  <c:v>07/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>06-01-2020</c:v>
+                  <c:v>06/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>03-01-2020</c:v>
+                  <c:v>03/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>02-01-2020</c:v>
+                  <c:v>02/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>31-12-2019</c:v>
+                  <c:v>31/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>30-12-2019</c:v>
+                  <c:v>30/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>27-12-2019</c:v>
+                  <c:v>27/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>24-12-2019</c:v>
+                  <c:v>24/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>23-12-2019</c:v>
+                  <c:v>23/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>20-12-2019</c:v>
+                  <c:v>20/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>19-12-2019</c:v>
+                  <c:v>19/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>18-12-2019</c:v>
+                  <c:v>18/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>17-12-2019</c:v>
+                  <c:v>17/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>16-12-2019</c:v>
+                  <c:v>16/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>13-12-2019</c:v>
+                  <c:v>13/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>12-12-2019</c:v>
+                  <c:v>12/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>11-12-2019</c:v>
+                  <c:v>11/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>10-12-2019</c:v>
+                  <c:v>10/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>09-12-2019</c:v>
+                  <c:v>09/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>06-12-2019</c:v>
+                  <c:v>06/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>05-12-2019</c:v>
+                  <c:v>05/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>04-12-2019</c:v>
+                  <c:v>04/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>03-12-2019</c:v>
+                  <c:v>03/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>02-12-2019</c:v>
+                  <c:v>02/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>29-11-2019</c:v>
+                  <c:v>29/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>28-11-2019</c:v>
+                  <c:v>28/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>27-11-2019</c:v>
+                  <c:v>27/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>26-11-2019</c:v>
+                  <c:v>26/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>25-11-2019</c:v>
+                  <c:v>25/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>22-11-2019</c:v>
+                  <c:v>22/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>21-11-2019</c:v>
+                  <c:v>21/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>20-11-2019</c:v>
+                  <c:v>20/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>19-11-2019</c:v>
+                  <c:v>19/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>18-11-2019</c:v>
+                  <c:v>18/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>15-11-2019</c:v>
+                  <c:v>15/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>14-11-2019</c:v>
+                  <c:v>14/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>13-11-2019</c:v>
+                  <c:v>13/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>12-11-2019</c:v>
+                  <c:v>12/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>11-11-2019</c:v>
+                  <c:v>11/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>08-11-2019</c:v>
+                  <c:v>08/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>07-11-2019</c:v>
+                  <c:v>07/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>06-11-2019</c:v>
+                  <c:v>06/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>05-11-2019</c:v>
+                  <c:v>05/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>04-11-2019</c:v>
+                  <c:v>04/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>01-11-2019</c:v>
+                  <c:v>01/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>31-10-2019</c:v>
+                  <c:v>31/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>30-10-2019</c:v>
+                  <c:v>30/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>29-10-2019</c:v>
+                  <c:v>29/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>28-10-2019</c:v>
+                  <c:v>28/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>25-10-2019</c:v>
+                  <c:v>25/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>24-10-2019</c:v>
+                  <c:v>24/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>23-10-2019</c:v>
+                  <c:v>23/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>22-10-2019</c:v>
+                  <c:v>22/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>21-10-2019</c:v>
+                  <c:v>21/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>18-10-2019</c:v>
+                  <c:v>18/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>17-10-2019</c:v>
+                  <c:v>17/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>16-10-2019</c:v>
+                  <c:v>16/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>15-10-2019</c:v>
+                  <c:v>15/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>14-10-2019</c:v>
+                  <c:v>14/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>11-10-2019</c:v>
+                  <c:v>11/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>10-10-2019</c:v>
+                  <c:v>10/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>09-10-2019</c:v>
+                  <c:v>09/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>08-10-2019</c:v>
+                  <c:v>08/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>07-10-2019</c:v>
+                  <c:v>07/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>04-10-2019</c:v>
+                  <c:v>04/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>03-10-2019</c:v>
+                  <c:v>03/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>02-10-2019</c:v>
+                  <c:v>02/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>01-10-2019</c:v>
+                  <c:v>01/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>30-09-2019</c:v>
+                  <c:v>30/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>27-09-2019</c:v>
+                  <c:v>27/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>26-09-2019</c:v>
+                  <c:v>26/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>25-09-2019</c:v>
+                  <c:v>25/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>24-09-2019</c:v>
+                  <c:v>24/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>23-09-2019</c:v>
+                  <c:v>23/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>20-09-2019</c:v>
+                  <c:v>20/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>19-09-2019</c:v>
+                  <c:v>19/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>18-09-2019</c:v>
+                  <c:v>18/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>17-09-2019</c:v>
+                  <c:v>17/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>16-09-2019</c:v>
+                  <c:v>16/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>13-09-2019</c:v>
+                  <c:v>13/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>12-09-2019</c:v>
+                  <c:v>12/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>11-09-2019</c:v>
+                  <c:v>11/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>10-09-2019</c:v>
+                  <c:v>10/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>09-09-2019</c:v>
+                  <c:v>09/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>06-09-2019</c:v>
+                  <c:v>06/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>05-09-2019</c:v>
+                  <c:v>05/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>04-09-2019</c:v>
+                  <c:v>04/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>03-09-2019</c:v>
+                  <c:v>03/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>02-09-2019</c:v>
+                  <c:v>02/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>30-08-2019</c:v>
+                  <c:v>30/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>29-08-2019</c:v>
+                  <c:v>29/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>28-08-2019</c:v>
+                  <c:v>28/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>27-08-2019</c:v>
+                  <c:v>27/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>23-08-2019</c:v>
+                  <c:v>23/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>22-08-2019</c:v>
+                  <c:v>22/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>21-08-2019</c:v>
+                  <c:v>21/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>20-08-2019</c:v>
+                  <c:v>20/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>19-08-2019</c:v>
+                  <c:v>19/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>16-08-2019</c:v>
+                  <c:v>16/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>15-08-2019</c:v>
+                  <c:v>15/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>14-08-2019</c:v>
+                  <c:v>14/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>13-08-2019</c:v>
+                  <c:v>13/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>12-08-2019</c:v>
+                  <c:v>12/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>09-08-2019</c:v>
+                  <c:v>09/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>08-08-2019</c:v>
+                  <c:v>08/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>07-08-2019</c:v>
+                  <c:v>07/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>06-08-2019</c:v>
+                  <c:v>06/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>05-08-2019</c:v>
+                  <c:v>05/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>02-08-2019</c:v>
+                  <c:v>02/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>01-08-2019</c:v>
+                  <c:v>01/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>31-07-2019</c:v>
+                  <c:v>31/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>30-07-2019</c:v>
+                  <c:v>30/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>29-07-2019</c:v>
+                  <c:v>29/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>26-07-2019</c:v>
+                  <c:v>26/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>25-07-2019</c:v>
+                  <c:v>25/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>24-07-2019</c:v>
+                  <c:v>24/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>23-07-2019</c:v>
+                  <c:v>23/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>22-07-2019</c:v>
+                  <c:v>22/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>19-07-2019</c:v>
+                  <c:v>19/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>18-07-2019</c:v>
+                  <c:v>18/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="136">
-                  <c:v>17-07-2019</c:v>
+                  <c:v>17/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="137">
-                  <c:v>16-07-2019</c:v>
+                  <c:v>16/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="138">
-                  <c:v>15-07-2019</c:v>
+                  <c:v>15/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="139">
-                  <c:v>12-07-2019</c:v>
+                  <c:v>12/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>11-07-2019</c:v>
+                  <c:v>11/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="141">
-                  <c:v>10-07-2019</c:v>
+                  <c:v>10/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="142">
-                  <c:v>09-07-2019</c:v>
+                  <c:v>09/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>08-07-2019</c:v>
+                  <c:v>08/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="144">
-                  <c:v>05-07-2019</c:v>
+                  <c:v>05/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="145">
-                  <c:v>04-07-2019</c:v>
+                  <c:v>04/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="146">
-                  <c:v>03-07-2019</c:v>
+                  <c:v>03/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="147">
-                  <c:v>02-07-2019</c:v>
+                  <c:v>02/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="148">
-                  <c:v>01-07-2019</c:v>
+                  <c:v>01/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="149">
-                  <c:v>28-06-2019</c:v>
+                  <c:v>28/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="150">
-                  <c:v>27-06-2019</c:v>
+                  <c:v>27/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="151">
-                  <c:v>26-06-2019</c:v>
+                  <c:v>26/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="152">
-                  <c:v>25-06-2019</c:v>
+                  <c:v>25/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="153">
-                  <c:v>24-06-2019</c:v>
+                  <c:v>24/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="154">
-                  <c:v>21-06-2019</c:v>
+                  <c:v>21/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="155">
-                  <c:v>20-06-2019</c:v>
+                  <c:v>20/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="156">
-                  <c:v>19-06-2019</c:v>
+                  <c:v>19/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="157">
-                  <c:v>18-06-2019</c:v>
+                  <c:v>18/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="158">
-                  <c:v>17-06-2019</c:v>
+                  <c:v>17/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="159">
-                  <c:v>14-06-2019</c:v>
+                  <c:v>14/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="160">
-                  <c:v>13-06-2019</c:v>
+                  <c:v>13/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="161">
-                  <c:v>12-06-2019</c:v>
+                  <c:v>12/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="162">
-                  <c:v>11-06-2019</c:v>
+                  <c:v>11/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="163">
-                  <c:v>10-06-2019</c:v>
+                  <c:v>10/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="164">
-                  <c:v>07-06-2019</c:v>
+                  <c:v>07/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="165">
-                  <c:v>06-06-2019</c:v>
+                  <c:v>06/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="166">
-                  <c:v>05-06-2019</c:v>
+                  <c:v>05/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="167">
-                  <c:v>04-06-2019</c:v>
+                  <c:v>04/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="168">
-                  <c:v>03-06-2019</c:v>
+                  <c:v>03/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="169">
-                  <c:v>31-05-2019</c:v>
+                  <c:v>31/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="170">
-                  <c:v>30-05-2019</c:v>
+                  <c:v>30/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="171">
-                  <c:v>29-05-2019</c:v>
+                  <c:v>29/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="172">
-                  <c:v>28-05-2019</c:v>
+                  <c:v>28/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="173">
-                  <c:v>24-05-2019</c:v>
+                  <c:v>24/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="174">
-                  <c:v>23-05-2019</c:v>
+                  <c:v>23/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="175">
-                  <c:v>22-05-2019</c:v>
+                  <c:v>22/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="176">
-                  <c:v>21-05-2019</c:v>
+                  <c:v>21/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="177">
-                  <c:v>20-05-2019</c:v>
+                  <c:v>20/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="178">
-                  <c:v>17-05-2019</c:v>
+                  <c:v>17/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="179">
-                  <c:v>16-05-2019</c:v>
+                  <c:v>16/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="180">
-                  <c:v>15-05-2019</c:v>
+                  <c:v>15/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="181">
-                  <c:v>14-05-2019</c:v>
+                  <c:v>14/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="182">
-                  <c:v>13-05-2019</c:v>
+                  <c:v>13/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="183">
-                  <c:v>10-05-2019</c:v>
+                  <c:v>10/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="184">
-                  <c:v>09-05-2019</c:v>
+                  <c:v>09/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="185">
-                  <c:v>08-05-2019</c:v>
+                  <c:v>08/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="186">
-                  <c:v>07-05-2019</c:v>
+                  <c:v>07/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="187">
-                  <c:v>03-05-2019</c:v>
+                  <c:v>03/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="188">
-                  <c:v>02-05-2019</c:v>
+                  <c:v>02/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="189">
-                  <c:v>01-05-2019</c:v>
+                  <c:v>01/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="190">
-                  <c:v>30-04-2019</c:v>
+                  <c:v>30/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="191">
-                  <c:v>29-04-2019</c:v>
+                  <c:v>29/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="192">
-                  <c:v>26-04-2019</c:v>
+                  <c:v>26/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="193">
-                  <c:v>25-04-2019</c:v>
+                  <c:v>25/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="194">
-                  <c:v>24-04-2019</c:v>
+                  <c:v>24/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="195">
-                  <c:v>23-04-2019</c:v>
+                  <c:v>23/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="196">
-                  <c:v>18-04-2019</c:v>
+                  <c:v>18/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="197">
-                  <c:v>17-04-2019</c:v>
+                  <c:v>17/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="198">
-                  <c:v>16-04-2019</c:v>
+                  <c:v>16/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="199">
-                  <c:v>15-04-2019</c:v>
+                  <c:v>15/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="200">
-                  <c:v>12-04-2019</c:v>
+                  <c:v>12/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="201">
-                  <c:v>11-04-2019</c:v>
+                  <c:v>11/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="202">
-                  <c:v>10-04-2019</c:v>
+                  <c:v>10/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="203">
-                  <c:v>09-04-2019</c:v>
+                  <c:v>09/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="204">
-                  <c:v>08-04-2019</c:v>
+                  <c:v>08/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="205">
-                  <c:v>05-04-2019</c:v>
+                  <c:v>05/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="206">
-                  <c:v>04-04-2019</c:v>
+                  <c:v>04/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="207">
-                  <c:v>03-04-2019</c:v>
+                  <c:v>03/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="208">
-                  <c:v>02-04-2019</c:v>
+                  <c:v>02/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="209">
-                  <c:v>01-04-2019</c:v>
+                  <c:v>01/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="210">
-                  <c:v>29-03-2019</c:v>
+                  <c:v>29/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="211">
-                  <c:v>28-03-2019</c:v>
+                  <c:v>28/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="212">
-                  <c:v>27-03-2019</c:v>
+                  <c:v>27/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="213">
-                  <c:v>26-03-2019</c:v>
+                  <c:v>26/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="214">
-                  <c:v>25-03-2019</c:v>
+                  <c:v>25/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="215">
-                  <c:v>22-03-2019</c:v>
+                  <c:v>22/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="216">
-                  <c:v>21-03-2019</c:v>
+                  <c:v>21/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="217">
-                  <c:v>20-03-2019</c:v>
+                  <c:v>20/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="218">
-                  <c:v>19-03-2019</c:v>
+                  <c:v>19/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="219">
-                  <c:v>18-03-2019</c:v>
+                  <c:v>18/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="220">
-                  <c:v>15-03-2019</c:v>
+                  <c:v>15/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="221">
-                  <c:v>14-03-2019</c:v>
+                  <c:v>14/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="222">
-                  <c:v>13-03-2019</c:v>
+                  <c:v>13/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="223">
-                  <c:v>12-03-2019</c:v>
+                  <c:v>12/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="224">
-                  <c:v>11-03-2019</c:v>
+                  <c:v>11/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="225">
-                  <c:v>08-03-2019</c:v>
+                  <c:v>08/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="226">
-                  <c:v>07-03-2019</c:v>
+                  <c:v>07/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="227">
-                  <c:v>06-03-2019</c:v>
+                  <c:v>06/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="228">
-                  <c:v>05-03-2019</c:v>
+                  <c:v>05/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="229">
-                  <c:v>04-03-2019</c:v>
+                  <c:v>04/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="230">
-                  <c:v>01-03-2019</c:v>
+                  <c:v>01/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="231">
-                  <c:v>28-02-2019</c:v>
+                  <c:v>28/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="232">
-                  <c:v>27-02-2019</c:v>
+                  <c:v>27/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="233">
-                  <c:v>26-02-2019</c:v>
+                  <c:v>26/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="234">
-                  <c:v>25-02-2019</c:v>
+                  <c:v>25/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="235">
-                  <c:v>22-02-2019</c:v>
+                  <c:v>22/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="236">
-                  <c:v>21-02-2019</c:v>
+                  <c:v>21/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="237">
-                  <c:v>20-02-2019</c:v>
+                  <c:v>20/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="238">
-                  <c:v>19-02-2019</c:v>
+                  <c:v>19/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="239">
-                  <c:v>18-02-2019</c:v>
+                  <c:v>18/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="240">
-                  <c:v>15-02-2019</c:v>
+                  <c:v>15/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="241">
-                  <c:v>14-02-2019</c:v>
+                  <c:v>14/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="242">
-                  <c:v>13-02-2019</c:v>
+                  <c:v>13/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="243">
-                  <c:v>12-02-2019</c:v>
+                  <c:v>12/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="244">
-                  <c:v>11-02-2019</c:v>
+                  <c:v>11/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="245">
-                  <c:v>08-02-2019</c:v>
+                  <c:v>08/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="246">
-                  <c:v>07-02-2019</c:v>
+                  <c:v>07/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="247">
-                  <c:v>06-02-2019</c:v>
+                  <c:v>06/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="248">
-                  <c:v>05-02-2019</c:v>
+                  <c:v>05/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="249">
-                  <c:v>04-02-2019</c:v>
+                  <c:v>04/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="250">
-                  <c:v>01-02-2019</c:v>
+                  <c:v>01/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="251">
-                  <c:v>31-01-2019</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="252">
-                  <c:v>30-01-2019</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="253">
-                  <c:v>29-01-2019</c:v>
-                </c:pt>
-                <c:pt idx="254">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="255">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="256">
                   <c:v/>
                 </c:pt>
               </c:strCache>
@@ -3438,10 +3402,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'pump.chart.data'!$C$2:$C$258</c:f>
+              <c:f>'pump.chart.data'!$C$2:$C$255</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="257"/>
+                <c:ptCount val="254"/>
                 <c:pt idx="0">
                   <c:v>132.53</c:v>
                 </c:pt>
@@ -4194,24 +4158,6 @@
                 </c:pt>
                 <c:pt idx="250">
                   <c:v>128.73</c:v>
-                </c:pt>
-                <c:pt idx="251">
-                  <c:v>128.72</c:v>
-                </c:pt>
-                <c:pt idx="252">
-                  <c:v>128.73</c:v>
-                </c:pt>
-                <c:pt idx="253">
-                  <c:v>128.81</c:v>
-                </c:pt>
-                <c:pt idx="254">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="255">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="256">
-                  <c:v/>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4226,11 +4172,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="2381999"/>
-        <c:axId val="21891262"/>
+        <c:axId val="95364165"/>
+        <c:axId val="10598239"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2381999"/>
+        <c:axId val="95364165"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4258,14 +4204,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="21891262"/>
+        <c:crossAx val="10598239"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="21891262"/>
+        <c:axId val="10598239"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4300,7 +4246,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2381999"/>
+        <c:crossAx val="95364165"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4339,7 +4285,7 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
@@ -4357,10 +4303,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0755925940485082"/>
-          <c:y val="0.0720247711362413"/>
-          <c:w val="0.898227131569637"/>
-          <c:h val="0.758952611739365"/>
+          <c:x val="0.0755955656891265"/>
+          <c:y val="0.0720296196566813"/>
+          <c:w val="0.898183819482664"/>
+          <c:h val="0.758869067653989"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -4418,778 +4364,769 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'oil.chart.data'!$A$2:$A$258</c:f>
+              <c:f>'oil.chart.data'!$A$2:$A$255</c:f>
               <c:strCache>
-                <c:ptCount val="257"/>
+                <c:ptCount val="254"/>
                 <c:pt idx="0">
-                  <c:v>29-01-2020</c:v>
+                  <c:v>29/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>28-01-2020</c:v>
+                  <c:v>28/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>27-01-2020</c:v>
+                  <c:v>27/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24-01-2020</c:v>
+                  <c:v>24/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23-01-2020</c:v>
+                  <c:v>23/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>22-01-2020</c:v>
+                  <c:v>22/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21-01-2020</c:v>
+                  <c:v>21/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>20-01-2020</c:v>
+                  <c:v>20/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>17-01-2020</c:v>
+                  <c:v>17/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>16-01-2020</c:v>
+                  <c:v>16/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>15-01-2020</c:v>
+                  <c:v>15/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>14-01-2020</c:v>
+                  <c:v>14/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>13-01-2020</c:v>
+                  <c:v>13/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>10-01-2020</c:v>
+                  <c:v>10/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>09-01-2020</c:v>
+                  <c:v>09/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>08-01-2020</c:v>
+                  <c:v>08/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>07-01-2020</c:v>
+                  <c:v>07/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>06-01-2020</c:v>
+                  <c:v>06/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>03-01-2020</c:v>
+                  <c:v>03/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>02-01-2020</c:v>
+                  <c:v>02/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>31-12-2019</c:v>
+                  <c:v>31/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>30-12-2019</c:v>
+                  <c:v>30/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>27-12-2019</c:v>
+                  <c:v>27/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>24-12-2019</c:v>
+                  <c:v>24/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>23-12-2019</c:v>
+                  <c:v>23/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>20-12-2019</c:v>
+                  <c:v>20/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>19-12-2019</c:v>
+                  <c:v>19/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>18-12-2019</c:v>
+                  <c:v>18/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>17-12-2019</c:v>
+                  <c:v>17/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>16-12-2019</c:v>
+                  <c:v>16/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>13-12-2019</c:v>
+                  <c:v>13/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>12-12-2019</c:v>
+                  <c:v>12/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>11-12-2019</c:v>
+                  <c:v>11/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>10-12-2019</c:v>
+                  <c:v>10/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>09-12-2019</c:v>
+                  <c:v>09/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>06-12-2019</c:v>
+                  <c:v>06/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>05-12-2019</c:v>
+                  <c:v>05/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>04-12-2019</c:v>
+                  <c:v>04/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>03-12-2019</c:v>
+                  <c:v>03/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>02-12-2019</c:v>
+                  <c:v>02/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>29-11-2019</c:v>
+                  <c:v>29/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>28-11-2019</c:v>
+                  <c:v>28/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>27-11-2019</c:v>
+                  <c:v>27/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>26-11-2019</c:v>
+                  <c:v>26/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>25-11-2019</c:v>
+                  <c:v>25/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>22-11-2019</c:v>
+                  <c:v>22/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>21-11-2019</c:v>
+                  <c:v>21/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>20-11-2019</c:v>
+                  <c:v>20/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>19-11-2019</c:v>
+                  <c:v>19/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>18-11-2019</c:v>
+                  <c:v>18/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>15-11-2019</c:v>
+                  <c:v>15/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>14-11-2019</c:v>
+                  <c:v>14/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>13-11-2019</c:v>
+                  <c:v>13/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>12-11-2019</c:v>
+                  <c:v>12/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>11-11-2019</c:v>
+                  <c:v>11/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>08-11-2019</c:v>
+                  <c:v>08/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>07-11-2019</c:v>
+                  <c:v>07/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>06-11-2019</c:v>
+                  <c:v>06/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>05-11-2019</c:v>
+                  <c:v>05/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>04-11-2019</c:v>
+                  <c:v>04/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>01-11-2019</c:v>
+                  <c:v>01/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>31-10-2019</c:v>
+                  <c:v>31/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>30-10-2019</c:v>
+                  <c:v>30/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>29-10-2019</c:v>
+                  <c:v>29/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>28-10-2019</c:v>
+                  <c:v>28/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>25-10-2019</c:v>
+                  <c:v>25/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>24-10-2019</c:v>
+                  <c:v>24/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>23-10-2019</c:v>
+                  <c:v>23/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>22-10-2019</c:v>
+                  <c:v>22/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>21-10-2019</c:v>
+                  <c:v>21/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>18-10-2019</c:v>
+                  <c:v>18/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>17-10-2019</c:v>
+                  <c:v>17/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>16-10-2019</c:v>
+                  <c:v>16/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>15-10-2019</c:v>
+                  <c:v>15/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>14-10-2019</c:v>
+                  <c:v>14/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>11-10-2019</c:v>
+                  <c:v>11/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>10-10-2019</c:v>
+                  <c:v>10/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>09-10-2019</c:v>
+                  <c:v>09/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>08-10-2019</c:v>
+                  <c:v>08/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>07-10-2019</c:v>
+                  <c:v>07/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>04-10-2019</c:v>
+                  <c:v>04/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>03-10-2019</c:v>
+                  <c:v>03/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>02-10-2019</c:v>
+                  <c:v>02/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>01-10-2019</c:v>
+                  <c:v>01/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>30-09-2019</c:v>
+                  <c:v>30/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>27-09-2019</c:v>
+                  <c:v>27/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>26-09-2019</c:v>
+                  <c:v>26/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>25-09-2019</c:v>
+                  <c:v>25/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>24-09-2019</c:v>
+                  <c:v>24/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>23-09-2019</c:v>
+                  <c:v>23/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>20-09-2019</c:v>
+                  <c:v>20/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>19-09-2019</c:v>
+                  <c:v>19/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>18-09-2019</c:v>
+                  <c:v>18/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>17-09-2019</c:v>
+                  <c:v>17/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>16-09-2019</c:v>
+                  <c:v>16/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>13-09-2019</c:v>
+                  <c:v>13/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>12-09-2019</c:v>
+                  <c:v>12/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>11-09-2019</c:v>
+                  <c:v>11/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>10-09-2019</c:v>
+                  <c:v>10/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>09-09-2019</c:v>
+                  <c:v>09/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>06-09-2019</c:v>
+                  <c:v>06/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>05-09-2019</c:v>
+                  <c:v>05/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>04-09-2019</c:v>
+                  <c:v>04/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>03-09-2019</c:v>
+                  <c:v>03/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>02-09-2019</c:v>
+                  <c:v>02/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>30-08-2019</c:v>
+                  <c:v>30/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>29-08-2019</c:v>
+                  <c:v>29/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>28-08-2019</c:v>
+                  <c:v>28/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>27-08-2019</c:v>
+                  <c:v>27/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>23-08-2019</c:v>
+                  <c:v>23/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>22-08-2019</c:v>
+                  <c:v>22/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>21-08-2019</c:v>
+                  <c:v>21/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>20-08-2019</c:v>
+                  <c:v>20/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>19-08-2019</c:v>
+                  <c:v>19/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>16-08-2019</c:v>
+                  <c:v>16/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>15-08-2019</c:v>
+                  <c:v>15/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>14-08-2019</c:v>
+                  <c:v>14/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>13-08-2019</c:v>
+                  <c:v>13/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>12-08-2019</c:v>
+                  <c:v>12/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>09-08-2019</c:v>
+                  <c:v>09/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>08-08-2019</c:v>
+                  <c:v>08/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>07-08-2019</c:v>
+                  <c:v>07/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>06-08-2019</c:v>
+                  <c:v>06/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>05-08-2019</c:v>
+                  <c:v>05/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>02-08-2019</c:v>
+                  <c:v>02/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>01-08-2019</c:v>
+                  <c:v>01/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>31-07-2019</c:v>
+                  <c:v>31/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>30-07-2019</c:v>
+                  <c:v>30/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>29-07-2019</c:v>
+                  <c:v>29/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>26-07-2019</c:v>
+                  <c:v>26/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>25-07-2019</c:v>
+                  <c:v>25/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>24-07-2019</c:v>
+                  <c:v>24/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>23-07-2019</c:v>
+                  <c:v>23/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>22-07-2019</c:v>
+                  <c:v>22/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>19-07-2019</c:v>
+                  <c:v>19/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>18-07-2019</c:v>
+                  <c:v>18/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="136">
-                  <c:v>17-07-2019</c:v>
+                  <c:v>17/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="137">
-                  <c:v>16-07-2019</c:v>
+                  <c:v>16/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="138">
-                  <c:v>15-07-2019</c:v>
+                  <c:v>15/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="139">
-                  <c:v>12-07-2019</c:v>
+                  <c:v>12/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>11-07-2019</c:v>
+                  <c:v>11/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="141">
-                  <c:v>10-07-2019</c:v>
+                  <c:v>10/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="142">
-                  <c:v>09-07-2019</c:v>
+                  <c:v>09/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>08-07-2019</c:v>
+                  <c:v>08/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="144">
-                  <c:v>05-07-2019</c:v>
+                  <c:v>05/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="145">
-                  <c:v>04-07-2019</c:v>
+                  <c:v>04/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="146">
-                  <c:v>03-07-2019</c:v>
+                  <c:v>03/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="147">
-                  <c:v>02-07-2019</c:v>
+                  <c:v>02/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="148">
-                  <c:v>01-07-2019</c:v>
+                  <c:v>01/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="149">
-                  <c:v>28-06-2019</c:v>
+                  <c:v>28/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="150">
-                  <c:v>27-06-2019</c:v>
+                  <c:v>27/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="151">
-                  <c:v>26-06-2019</c:v>
+                  <c:v>26/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="152">
-                  <c:v>25-06-2019</c:v>
+                  <c:v>25/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="153">
-                  <c:v>24-06-2019</c:v>
+                  <c:v>24/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="154">
-                  <c:v>21-06-2019</c:v>
+                  <c:v>21/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="155">
-                  <c:v>20-06-2019</c:v>
+                  <c:v>20/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="156">
-                  <c:v>19-06-2019</c:v>
+                  <c:v>19/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="157">
-                  <c:v>18-06-2019</c:v>
+                  <c:v>18/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="158">
-                  <c:v>17-06-2019</c:v>
+                  <c:v>17/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="159">
-                  <c:v>14-06-2019</c:v>
+                  <c:v>14/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="160">
-                  <c:v>13-06-2019</c:v>
+                  <c:v>13/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="161">
-                  <c:v>12-06-2019</c:v>
+                  <c:v>12/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="162">
-                  <c:v>11-06-2019</c:v>
+                  <c:v>11/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="163">
-                  <c:v>10-06-2019</c:v>
+                  <c:v>10/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="164">
-                  <c:v>07-06-2019</c:v>
+                  <c:v>07/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="165">
-                  <c:v>06-06-2019</c:v>
+                  <c:v>06/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="166">
-                  <c:v>05-06-2019</c:v>
+                  <c:v>05/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="167">
-                  <c:v>04-06-2019</c:v>
+                  <c:v>04/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="168">
-                  <c:v>03-06-2019</c:v>
+                  <c:v>03/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="169">
-                  <c:v>31-05-2019</c:v>
+                  <c:v>31/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="170">
-                  <c:v>30-05-2019</c:v>
+                  <c:v>30/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="171">
-                  <c:v>29-05-2019</c:v>
+                  <c:v>29/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="172">
-                  <c:v>28-05-2019</c:v>
+                  <c:v>28/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="173">
-                  <c:v>24-05-2019</c:v>
+                  <c:v>24/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="174">
-                  <c:v>23-05-2019</c:v>
+                  <c:v>23/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="175">
-                  <c:v>22-05-2019</c:v>
+                  <c:v>22/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="176">
-                  <c:v>21-05-2019</c:v>
+                  <c:v>21/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="177">
-                  <c:v>20-05-2019</c:v>
+                  <c:v>20/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="178">
-                  <c:v>17-05-2019</c:v>
+                  <c:v>17/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="179">
-                  <c:v>16-05-2019</c:v>
+                  <c:v>16/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="180">
-                  <c:v>15-05-2019</c:v>
+                  <c:v>15/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="181">
-                  <c:v>14-05-2019</c:v>
+                  <c:v>14/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="182">
-                  <c:v>13-05-2019</c:v>
+                  <c:v>13/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="183">
-                  <c:v>10-05-2019</c:v>
+                  <c:v>10/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="184">
-                  <c:v>09-05-2019</c:v>
+                  <c:v>09/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="185">
-                  <c:v>08-05-2019</c:v>
+                  <c:v>08/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="186">
-                  <c:v>07-05-2019</c:v>
+                  <c:v>07/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="187">
-                  <c:v>03-05-2019</c:v>
+                  <c:v>03/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="188">
-                  <c:v>02-05-2019</c:v>
+                  <c:v>02/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="189">
-                  <c:v>01-05-2019</c:v>
+                  <c:v>01/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="190">
-                  <c:v>30-04-2019</c:v>
+                  <c:v>30/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="191">
-                  <c:v>29-04-2019</c:v>
+                  <c:v>29/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="192">
-                  <c:v>26-04-2019</c:v>
+                  <c:v>26/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="193">
-                  <c:v>25-04-2019</c:v>
+                  <c:v>25/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="194">
-                  <c:v>24-04-2019</c:v>
+                  <c:v>24/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="195">
-                  <c:v>23-04-2019</c:v>
+                  <c:v>23/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="196">
-                  <c:v>18-04-2019</c:v>
+                  <c:v>18/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="197">
-                  <c:v>17-04-2019</c:v>
+                  <c:v>17/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="198">
-                  <c:v>16-04-2019</c:v>
+                  <c:v>16/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="199">
-                  <c:v>15-04-2019</c:v>
+                  <c:v>15/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="200">
-                  <c:v>12-04-2019</c:v>
+                  <c:v>12/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="201">
-                  <c:v>11-04-2019</c:v>
+                  <c:v>11/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="202">
-                  <c:v>10-04-2019</c:v>
+                  <c:v>10/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="203">
-                  <c:v>09-04-2019</c:v>
+                  <c:v>09/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="204">
-                  <c:v>08-04-2019</c:v>
+                  <c:v>08/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="205">
-                  <c:v>05-04-2019</c:v>
+                  <c:v>05/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="206">
-                  <c:v>04-04-2019</c:v>
+                  <c:v>04/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="207">
-                  <c:v>03-04-2019</c:v>
+                  <c:v>03/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="208">
-                  <c:v>02-04-2019</c:v>
+                  <c:v>02/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="209">
-                  <c:v>01-04-2019</c:v>
+                  <c:v>01/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="210">
-                  <c:v>29-03-2019</c:v>
+                  <c:v>29/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="211">
-                  <c:v>28-03-2019</c:v>
+                  <c:v>28/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="212">
-                  <c:v>27-03-2019</c:v>
+                  <c:v>27/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="213">
-                  <c:v>26-03-2019</c:v>
+                  <c:v>26/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="214">
-                  <c:v>25-03-2019</c:v>
+                  <c:v>25/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="215">
-                  <c:v>22-03-2019</c:v>
+                  <c:v>22/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="216">
-                  <c:v>21-03-2019</c:v>
+                  <c:v>21/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="217">
-                  <c:v>20-03-2019</c:v>
+                  <c:v>20/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="218">
-                  <c:v>19-03-2019</c:v>
+                  <c:v>19/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="219">
-                  <c:v>18-03-2019</c:v>
+                  <c:v>18/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="220">
-                  <c:v>15-03-2019</c:v>
+                  <c:v>15/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="221">
-                  <c:v>14-03-2019</c:v>
+                  <c:v>14/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="222">
-                  <c:v>13-03-2019</c:v>
+                  <c:v>13/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="223">
-                  <c:v>12-03-2019</c:v>
+                  <c:v>12/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="224">
-                  <c:v>11-03-2019</c:v>
+                  <c:v>11/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="225">
-                  <c:v>08-03-2019</c:v>
+                  <c:v>08/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="226">
-                  <c:v>07-03-2019</c:v>
+                  <c:v>07/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="227">
-                  <c:v>06-03-2019</c:v>
+                  <c:v>06/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="228">
-                  <c:v>05-03-2019</c:v>
+                  <c:v>05/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="229">
-                  <c:v>04-03-2019</c:v>
+                  <c:v>04/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="230">
-                  <c:v>01-03-2019</c:v>
+                  <c:v>01/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="231">
-                  <c:v>28-02-2019</c:v>
+                  <c:v>28/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="232">
-                  <c:v>27-02-2019</c:v>
+                  <c:v>27/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="233">
-                  <c:v>26-02-2019</c:v>
+                  <c:v>26/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="234">
-                  <c:v>25-02-2019</c:v>
+                  <c:v>25/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="235">
-                  <c:v>22-02-2019</c:v>
+                  <c:v>22/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="236">
-                  <c:v>21-02-2019</c:v>
+                  <c:v>21/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="237">
-                  <c:v>20-02-2019</c:v>
+                  <c:v>20/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="238">
-                  <c:v>19-02-2019</c:v>
+                  <c:v>19/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="239">
-                  <c:v>18-02-2019</c:v>
+                  <c:v>18/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="240">
-                  <c:v>15-02-2019</c:v>
+                  <c:v>15/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="241">
-                  <c:v>14-02-2019</c:v>
+                  <c:v>14/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="242">
-                  <c:v>13-02-2019</c:v>
+                  <c:v>13/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="243">
-                  <c:v>12-02-2019</c:v>
+                  <c:v>12/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="244">
-                  <c:v>11-02-2019</c:v>
+                  <c:v>11/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="245">
-                  <c:v>08-02-2019</c:v>
+                  <c:v>08/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="246">
-                  <c:v>07-02-2019</c:v>
+                  <c:v>07/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="247">
-                  <c:v>06-02-2019</c:v>
+                  <c:v>06/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="248">
-                  <c:v>05-02-2019</c:v>
+                  <c:v>05/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="249">
-                  <c:v>04-02-2019</c:v>
+                  <c:v>04/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="250">
-                  <c:v>01-02-2019</c:v>
+                  <c:v>01/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="251">
-                  <c:v>31-01-2019</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="252">
-                  <c:v>30-01-2019</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="253">
-                  <c:v>29-01-2019</c:v>
-                </c:pt>
-                <c:pt idx="254">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="255">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="256">
                   <c:v/>
                 </c:pt>
               </c:strCache>
@@ -5197,10 +5134,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'oil.chart.data'!$B$2:$B$258</c:f>
+              <c:f>'oil.chart.data'!$B$2:$B$255</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="257"/>
+                <c:ptCount val="254"/>
                 <c:pt idx="0">
                   <c:v>59.37</c:v>
                 </c:pt>
@@ -5953,24 +5890,6 @@
                 </c:pt>
                 <c:pt idx="250">
                   <c:v>62.05</c:v>
-                </c:pt>
-                <c:pt idx="251">
-                  <c:v>62.26</c:v>
-                </c:pt>
-                <c:pt idx="252">
-                  <c:v>62.4</c:v>
-                </c:pt>
-                <c:pt idx="253">
-                  <c:v>61.45</c:v>
-                </c:pt>
-                <c:pt idx="254">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="255">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="256">
-                  <c:v/>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6029,778 +5948,769 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'oil.chart.data'!$A$2:$A$258</c:f>
+              <c:f>'oil.chart.data'!$A$2:$A$255</c:f>
               <c:strCache>
-                <c:ptCount val="257"/>
+                <c:ptCount val="254"/>
                 <c:pt idx="0">
-                  <c:v>29-01-2020</c:v>
+                  <c:v>29/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>28-01-2020</c:v>
+                  <c:v>28/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>27-01-2020</c:v>
+                  <c:v>27/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24-01-2020</c:v>
+                  <c:v>24/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23-01-2020</c:v>
+                  <c:v>23/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>22-01-2020</c:v>
+                  <c:v>22/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21-01-2020</c:v>
+                  <c:v>21/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>20-01-2020</c:v>
+                  <c:v>20/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>17-01-2020</c:v>
+                  <c:v>17/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>16-01-2020</c:v>
+                  <c:v>16/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>15-01-2020</c:v>
+                  <c:v>15/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>14-01-2020</c:v>
+                  <c:v>14/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>13-01-2020</c:v>
+                  <c:v>13/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>10-01-2020</c:v>
+                  <c:v>10/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>09-01-2020</c:v>
+                  <c:v>09/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>08-01-2020</c:v>
+                  <c:v>08/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>07-01-2020</c:v>
+                  <c:v>07/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>06-01-2020</c:v>
+                  <c:v>06/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>03-01-2020</c:v>
+                  <c:v>03/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>02-01-2020</c:v>
+                  <c:v>02/01/2020</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>31-12-2019</c:v>
+                  <c:v>31/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>30-12-2019</c:v>
+                  <c:v>30/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>27-12-2019</c:v>
+                  <c:v>27/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>24-12-2019</c:v>
+                  <c:v>24/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>23-12-2019</c:v>
+                  <c:v>23/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>20-12-2019</c:v>
+                  <c:v>20/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>19-12-2019</c:v>
+                  <c:v>19/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>18-12-2019</c:v>
+                  <c:v>18/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>17-12-2019</c:v>
+                  <c:v>17/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>16-12-2019</c:v>
+                  <c:v>16/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>13-12-2019</c:v>
+                  <c:v>13/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>12-12-2019</c:v>
+                  <c:v>12/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>11-12-2019</c:v>
+                  <c:v>11/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>10-12-2019</c:v>
+                  <c:v>10/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>09-12-2019</c:v>
+                  <c:v>09/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>06-12-2019</c:v>
+                  <c:v>06/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>05-12-2019</c:v>
+                  <c:v>05/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>04-12-2019</c:v>
+                  <c:v>04/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>03-12-2019</c:v>
+                  <c:v>03/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>02-12-2019</c:v>
+                  <c:v>02/12/2019</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>29-11-2019</c:v>
+                  <c:v>29/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>28-11-2019</c:v>
+                  <c:v>28/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>27-11-2019</c:v>
+                  <c:v>27/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>26-11-2019</c:v>
+                  <c:v>26/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>25-11-2019</c:v>
+                  <c:v>25/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>22-11-2019</c:v>
+                  <c:v>22/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>21-11-2019</c:v>
+                  <c:v>21/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>20-11-2019</c:v>
+                  <c:v>20/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>19-11-2019</c:v>
+                  <c:v>19/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>18-11-2019</c:v>
+                  <c:v>18/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>15-11-2019</c:v>
+                  <c:v>15/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>14-11-2019</c:v>
+                  <c:v>14/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>13-11-2019</c:v>
+                  <c:v>13/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>12-11-2019</c:v>
+                  <c:v>12/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>11-11-2019</c:v>
+                  <c:v>11/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>08-11-2019</c:v>
+                  <c:v>08/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>07-11-2019</c:v>
+                  <c:v>07/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>06-11-2019</c:v>
+                  <c:v>06/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>05-11-2019</c:v>
+                  <c:v>05/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>04-11-2019</c:v>
+                  <c:v>04/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>01-11-2019</c:v>
+                  <c:v>01/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>31-10-2019</c:v>
+                  <c:v>31/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>30-10-2019</c:v>
+                  <c:v>30/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>29-10-2019</c:v>
+                  <c:v>29/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>28-10-2019</c:v>
+                  <c:v>28/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>25-10-2019</c:v>
+                  <c:v>25/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>24-10-2019</c:v>
+                  <c:v>24/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>23-10-2019</c:v>
+                  <c:v>23/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>22-10-2019</c:v>
+                  <c:v>22/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>21-10-2019</c:v>
+                  <c:v>21/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>18-10-2019</c:v>
+                  <c:v>18/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>17-10-2019</c:v>
+                  <c:v>17/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>16-10-2019</c:v>
+                  <c:v>16/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>15-10-2019</c:v>
+                  <c:v>15/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>14-10-2019</c:v>
+                  <c:v>14/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>11-10-2019</c:v>
+                  <c:v>11/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>10-10-2019</c:v>
+                  <c:v>10/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>09-10-2019</c:v>
+                  <c:v>09/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>08-10-2019</c:v>
+                  <c:v>08/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>07-10-2019</c:v>
+                  <c:v>07/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>04-10-2019</c:v>
+                  <c:v>04/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>03-10-2019</c:v>
+                  <c:v>03/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>02-10-2019</c:v>
+                  <c:v>02/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>01-10-2019</c:v>
+                  <c:v>01/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>30-09-2019</c:v>
+                  <c:v>30/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>27-09-2019</c:v>
+                  <c:v>27/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>26-09-2019</c:v>
+                  <c:v>26/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>25-09-2019</c:v>
+                  <c:v>25/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>24-09-2019</c:v>
+                  <c:v>24/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>23-09-2019</c:v>
+                  <c:v>23/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>20-09-2019</c:v>
+                  <c:v>20/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>19-09-2019</c:v>
+                  <c:v>19/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>18-09-2019</c:v>
+                  <c:v>18/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>17-09-2019</c:v>
+                  <c:v>17/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>16-09-2019</c:v>
+                  <c:v>16/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>13-09-2019</c:v>
+                  <c:v>13/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>12-09-2019</c:v>
+                  <c:v>12/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>11-09-2019</c:v>
+                  <c:v>11/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>10-09-2019</c:v>
+                  <c:v>10/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>09-09-2019</c:v>
+                  <c:v>09/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>06-09-2019</c:v>
+                  <c:v>06/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>05-09-2019</c:v>
+                  <c:v>05/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>04-09-2019</c:v>
+                  <c:v>04/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>03-09-2019</c:v>
+                  <c:v>03/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>02-09-2019</c:v>
+                  <c:v>02/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>30-08-2019</c:v>
+                  <c:v>30/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>29-08-2019</c:v>
+                  <c:v>29/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>28-08-2019</c:v>
+                  <c:v>28/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>27-08-2019</c:v>
+                  <c:v>27/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>23-08-2019</c:v>
+                  <c:v>23/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>22-08-2019</c:v>
+                  <c:v>22/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>21-08-2019</c:v>
+                  <c:v>21/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>20-08-2019</c:v>
+                  <c:v>20/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>19-08-2019</c:v>
+                  <c:v>19/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>16-08-2019</c:v>
+                  <c:v>16/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>15-08-2019</c:v>
+                  <c:v>15/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>14-08-2019</c:v>
+                  <c:v>14/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>13-08-2019</c:v>
+                  <c:v>13/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>12-08-2019</c:v>
+                  <c:v>12/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>09-08-2019</c:v>
+                  <c:v>09/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>08-08-2019</c:v>
+                  <c:v>08/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>07-08-2019</c:v>
+                  <c:v>07/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>06-08-2019</c:v>
+                  <c:v>06/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>05-08-2019</c:v>
+                  <c:v>05/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>02-08-2019</c:v>
+                  <c:v>02/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>01-08-2019</c:v>
+                  <c:v>01/08/2019</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>31-07-2019</c:v>
+                  <c:v>31/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>30-07-2019</c:v>
+                  <c:v>30/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>29-07-2019</c:v>
+                  <c:v>29/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>26-07-2019</c:v>
+                  <c:v>26/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>25-07-2019</c:v>
+                  <c:v>25/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>24-07-2019</c:v>
+                  <c:v>24/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>23-07-2019</c:v>
+                  <c:v>23/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>22-07-2019</c:v>
+                  <c:v>22/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>19-07-2019</c:v>
+                  <c:v>19/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>18-07-2019</c:v>
+                  <c:v>18/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="136">
-                  <c:v>17-07-2019</c:v>
+                  <c:v>17/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="137">
-                  <c:v>16-07-2019</c:v>
+                  <c:v>16/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="138">
-                  <c:v>15-07-2019</c:v>
+                  <c:v>15/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="139">
-                  <c:v>12-07-2019</c:v>
+                  <c:v>12/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>11-07-2019</c:v>
+                  <c:v>11/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="141">
-                  <c:v>10-07-2019</c:v>
+                  <c:v>10/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="142">
-                  <c:v>09-07-2019</c:v>
+                  <c:v>09/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>08-07-2019</c:v>
+                  <c:v>08/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="144">
-                  <c:v>05-07-2019</c:v>
+                  <c:v>05/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="145">
-                  <c:v>04-07-2019</c:v>
+                  <c:v>04/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="146">
-                  <c:v>03-07-2019</c:v>
+                  <c:v>03/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="147">
-                  <c:v>02-07-2019</c:v>
+                  <c:v>02/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="148">
-                  <c:v>01-07-2019</c:v>
+                  <c:v>01/07/2019</c:v>
                 </c:pt>
                 <c:pt idx="149">
-                  <c:v>28-06-2019</c:v>
+                  <c:v>28/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="150">
-                  <c:v>27-06-2019</c:v>
+                  <c:v>27/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="151">
-                  <c:v>26-06-2019</c:v>
+                  <c:v>26/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="152">
-                  <c:v>25-06-2019</c:v>
+                  <c:v>25/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="153">
-                  <c:v>24-06-2019</c:v>
+                  <c:v>24/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="154">
-                  <c:v>21-06-2019</c:v>
+                  <c:v>21/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="155">
-                  <c:v>20-06-2019</c:v>
+                  <c:v>20/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="156">
-                  <c:v>19-06-2019</c:v>
+                  <c:v>19/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="157">
-                  <c:v>18-06-2019</c:v>
+                  <c:v>18/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="158">
-                  <c:v>17-06-2019</c:v>
+                  <c:v>17/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="159">
-                  <c:v>14-06-2019</c:v>
+                  <c:v>14/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="160">
-                  <c:v>13-06-2019</c:v>
+                  <c:v>13/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="161">
-                  <c:v>12-06-2019</c:v>
+                  <c:v>12/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="162">
-                  <c:v>11-06-2019</c:v>
+                  <c:v>11/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="163">
-                  <c:v>10-06-2019</c:v>
+                  <c:v>10/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="164">
-                  <c:v>07-06-2019</c:v>
+                  <c:v>07/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="165">
-                  <c:v>06-06-2019</c:v>
+                  <c:v>06/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="166">
-                  <c:v>05-06-2019</c:v>
+                  <c:v>05/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="167">
-                  <c:v>04-06-2019</c:v>
+                  <c:v>04/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="168">
-                  <c:v>03-06-2019</c:v>
+                  <c:v>03/06/2019</c:v>
                 </c:pt>
                 <c:pt idx="169">
-                  <c:v>31-05-2019</c:v>
+                  <c:v>31/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="170">
-                  <c:v>30-05-2019</c:v>
+                  <c:v>30/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="171">
-                  <c:v>29-05-2019</c:v>
+                  <c:v>29/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="172">
-                  <c:v>28-05-2019</c:v>
+                  <c:v>28/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="173">
-                  <c:v>24-05-2019</c:v>
+                  <c:v>24/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="174">
-                  <c:v>23-05-2019</c:v>
+                  <c:v>23/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="175">
-                  <c:v>22-05-2019</c:v>
+                  <c:v>22/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="176">
-                  <c:v>21-05-2019</c:v>
+                  <c:v>21/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="177">
-                  <c:v>20-05-2019</c:v>
+                  <c:v>20/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="178">
-                  <c:v>17-05-2019</c:v>
+                  <c:v>17/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="179">
-                  <c:v>16-05-2019</c:v>
+                  <c:v>16/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="180">
-                  <c:v>15-05-2019</c:v>
+                  <c:v>15/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="181">
-                  <c:v>14-05-2019</c:v>
+                  <c:v>14/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="182">
-                  <c:v>13-05-2019</c:v>
+                  <c:v>13/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="183">
-                  <c:v>10-05-2019</c:v>
+                  <c:v>10/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="184">
-                  <c:v>09-05-2019</c:v>
+                  <c:v>09/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="185">
-                  <c:v>08-05-2019</c:v>
+                  <c:v>08/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="186">
-                  <c:v>07-05-2019</c:v>
+                  <c:v>07/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="187">
-                  <c:v>03-05-2019</c:v>
+                  <c:v>03/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="188">
-                  <c:v>02-05-2019</c:v>
+                  <c:v>02/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="189">
-                  <c:v>01-05-2019</c:v>
+                  <c:v>01/05/2019</c:v>
                 </c:pt>
                 <c:pt idx="190">
-                  <c:v>30-04-2019</c:v>
+                  <c:v>30/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="191">
-                  <c:v>29-04-2019</c:v>
+                  <c:v>29/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="192">
-                  <c:v>26-04-2019</c:v>
+                  <c:v>26/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="193">
-                  <c:v>25-04-2019</c:v>
+                  <c:v>25/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="194">
-                  <c:v>24-04-2019</c:v>
+                  <c:v>24/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="195">
-                  <c:v>23-04-2019</c:v>
+                  <c:v>23/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="196">
-                  <c:v>18-04-2019</c:v>
+                  <c:v>18/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="197">
-                  <c:v>17-04-2019</c:v>
+                  <c:v>17/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="198">
-                  <c:v>16-04-2019</c:v>
+                  <c:v>16/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="199">
-                  <c:v>15-04-2019</c:v>
+                  <c:v>15/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="200">
-                  <c:v>12-04-2019</c:v>
+                  <c:v>12/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="201">
-                  <c:v>11-04-2019</c:v>
+                  <c:v>11/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="202">
-                  <c:v>10-04-2019</c:v>
+                  <c:v>10/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="203">
-                  <c:v>09-04-2019</c:v>
+                  <c:v>09/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="204">
-                  <c:v>08-04-2019</c:v>
+                  <c:v>08/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="205">
-                  <c:v>05-04-2019</c:v>
+                  <c:v>05/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="206">
-                  <c:v>04-04-2019</c:v>
+                  <c:v>04/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="207">
-                  <c:v>03-04-2019</c:v>
+                  <c:v>03/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="208">
-                  <c:v>02-04-2019</c:v>
+                  <c:v>02/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="209">
-                  <c:v>01-04-2019</c:v>
+                  <c:v>01/04/2019</c:v>
                 </c:pt>
                 <c:pt idx="210">
-                  <c:v>29-03-2019</c:v>
+                  <c:v>29/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="211">
-                  <c:v>28-03-2019</c:v>
+                  <c:v>28/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="212">
-                  <c:v>27-03-2019</c:v>
+                  <c:v>27/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="213">
-                  <c:v>26-03-2019</c:v>
+                  <c:v>26/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="214">
-                  <c:v>25-03-2019</c:v>
+                  <c:v>25/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="215">
-                  <c:v>22-03-2019</c:v>
+                  <c:v>22/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="216">
-                  <c:v>21-03-2019</c:v>
+                  <c:v>21/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="217">
-                  <c:v>20-03-2019</c:v>
+                  <c:v>20/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="218">
-                  <c:v>19-03-2019</c:v>
+                  <c:v>19/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="219">
-                  <c:v>18-03-2019</c:v>
+                  <c:v>18/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="220">
-                  <c:v>15-03-2019</c:v>
+                  <c:v>15/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="221">
-                  <c:v>14-03-2019</c:v>
+                  <c:v>14/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="222">
-                  <c:v>13-03-2019</c:v>
+                  <c:v>13/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="223">
-                  <c:v>12-03-2019</c:v>
+                  <c:v>12/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="224">
-                  <c:v>11-03-2019</c:v>
+                  <c:v>11/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="225">
-                  <c:v>08-03-2019</c:v>
+                  <c:v>08/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="226">
-                  <c:v>07-03-2019</c:v>
+                  <c:v>07/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="227">
-                  <c:v>06-03-2019</c:v>
+                  <c:v>06/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="228">
-                  <c:v>05-03-2019</c:v>
+                  <c:v>05/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="229">
-                  <c:v>04-03-2019</c:v>
+                  <c:v>04/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="230">
-                  <c:v>01-03-2019</c:v>
+                  <c:v>01/03/2019</c:v>
                 </c:pt>
                 <c:pt idx="231">
-                  <c:v>28-02-2019</c:v>
+                  <c:v>28/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="232">
-                  <c:v>27-02-2019</c:v>
+                  <c:v>27/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="233">
-                  <c:v>26-02-2019</c:v>
+                  <c:v>26/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="234">
-                  <c:v>25-02-2019</c:v>
+                  <c:v>25/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="235">
-                  <c:v>22-02-2019</c:v>
+                  <c:v>22/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="236">
-                  <c:v>21-02-2019</c:v>
+                  <c:v>21/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="237">
-                  <c:v>20-02-2019</c:v>
+                  <c:v>20/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="238">
-                  <c:v>19-02-2019</c:v>
+                  <c:v>19/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="239">
-                  <c:v>18-02-2019</c:v>
+                  <c:v>18/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="240">
-                  <c:v>15-02-2019</c:v>
+                  <c:v>15/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="241">
-                  <c:v>14-02-2019</c:v>
+                  <c:v>14/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="242">
-                  <c:v>13-02-2019</c:v>
+                  <c:v>13/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="243">
-                  <c:v>12-02-2019</c:v>
+                  <c:v>12/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="244">
-                  <c:v>11-02-2019</c:v>
+                  <c:v>11/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="245">
-                  <c:v>08-02-2019</c:v>
+                  <c:v>08/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="246">
-                  <c:v>07-02-2019</c:v>
+                  <c:v>07/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="247">
-                  <c:v>06-02-2019</c:v>
+                  <c:v>06/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="248">
-                  <c:v>05-02-2019</c:v>
+                  <c:v>05/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="249">
-                  <c:v>04-02-2019</c:v>
+                  <c:v>04/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="250">
-                  <c:v>01-02-2019</c:v>
+                  <c:v>01/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="251">
-                  <c:v>31-01-2019</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="252">
-                  <c:v>30-01-2019</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="253">
-                  <c:v>29-01-2019</c:v>
-                </c:pt>
-                <c:pt idx="254">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="255">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="256">
                   <c:v/>
                 </c:pt>
               </c:strCache>
@@ -6808,10 +6718,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'oil.chart.data'!$C$2:$C$258</c:f>
+              <c:f>'oil.chart.data'!$C$2:$C$255</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="257"/>
+                <c:ptCount val="254"/>
                 <c:pt idx="0">
                   <c:v>45.66</c:v>
                 </c:pt>
@@ -7564,24 +7474,6 @@
                 </c:pt>
                 <c:pt idx="250">
                   <c:v>47.39</c:v>
-                </c:pt>
-                <c:pt idx="251">
-                  <c:v>47.33</c:v>
-                </c:pt>
-                <c:pt idx="252">
-                  <c:v>47.74</c:v>
-                </c:pt>
-                <c:pt idx="253">
-                  <c:v>46.74</c:v>
-                </c:pt>
-                <c:pt idx="254">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="255">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="256">
-                  <c:v/>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7596,11 +7488,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="58992009"/>
-        <c:axId val="57152822"/>
+        <c:axId val="52385031"/>
+        <c:axId val="66238166"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="58992009"/>
+        <c:axId val="52385031"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7628,14 +7520,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57152822"/>
+        <c:crossAx val="66238166"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="57152822"/>
+        <c:axId val="66238166"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7670,7 +7562,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="58992009"/>
+        <c:crossAx val="52385031"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7709,7 +7601,7 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
@@ -7721,9 +7613,9 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>40680</xdr:colOff>
+      <xdr:colOff>41040</xdr:colOff>
       <xdr:row>259</xdr:row>
-      <xdr:rowOff>57960</xdr:rowOff>
+      <xdr:rowOff>58320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
@@ -7737,8 +7629,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10731960" y="49012560"/>
-        <a:ext cx="5754960" cy="3234960"/>
+        <a:off x="10732320" y="48970800"/>
+        <a:ext cx="5754600" cy="3234600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7762,9 +7654,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>216000</xdr:colOff>
+      <xdr:colOff>215640</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>7560</xdr:rowOff>
+      <xdr:rowOff>7200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7773,7 +7665,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="29520" y="28800"/>
-        <a:ext cx="8314200" cy="4855320"/>
+        <a:ext cx="8313840" cy="4854960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7797,9 +7689,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>217440</xdr:colOff>
+      <xdr:colOff>217080</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>146520</xdr:rowOff>
+      <xdr:rowOff>146160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7808,7 +7700,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="360" y="360"/>
-        <a:ext cx="9157680" cy="5347800"/>
+        <a:ext cx="9157320" cy="5347440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7829,15 +7721,13 @@
   <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A:A"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="65.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="40.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8398,19 +8288,17 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A:A"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9009,17 +8897,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C255"/>
+  <dimension ref="A1:C252"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A:A"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A245" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A253" activeCellId="0" sqref="A253"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="11.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="7.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11792,39 +11679,6 @@
       </c>
       <c r="C252" s="2" t="n">
         <v>128.73</v>
-      </c>
-    </row>
-    <row r="253" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A253" s="4" t="n">
-        <v>43496.0416666667</v>
-      </c>
-      <c r="B253" s="2" t="n">
-        <v>119.65</v>
-      </c>
-      <c r="C253" s="2" t="n">
-        <v>128.72</v>
-      </c>
-    </row>
-    <row r="254" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A254" s="4" t="n">
-        <v>43495.0416666667</v>
-      </c>
-      <c r="B254" s="2" t="n">
-        <v>119.65</v>
-      </c>
-      <c r="C254" s="2" t="n">
-        <v>128.73</v>
-      </c>
-    </row>
-    <row r="255" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A255" s="4" t="n">
-        <v>43494.0416666667</v>
-      </c>
-      <c r="B255" s="2" t="n">
-        <v>119.82</v>
-      </c>
-      <c r="C255" s="2" t="n">
-        <v>128.81</v>
       </c>
     </row>
   </sheetData>
@@ -11843,17 +11697,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C255"/>
+  <dimension ref="A1:C252"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A:A"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A243" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A253" activeCellId="0" sqref="A253"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="11.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="24.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14626,39 +14479,6 @@
       </c>
       <c r="C252" s="2" t="n">
         <v>47.39</v>
-      </c>
-    </row>
-    <row r="253" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A253" s="4" t="n">
-        <v>43496.0416666667</v>
-      </c>
-      <c r="B253" s="2" t="n">
-        <v>62.26</v>
-      </c>
-      <c r="C253" s="2" t="n">
-        <v>47.33</v>
-      </c>
-    </row>
-    <row r="254" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A254" s="4" t="n">
-        <v>43495.0416666667</v>
-      </c>
-      <c r="B254" s="2" t="n">
-        <v>62.4</v>
-      </c>
-      <c r="C254" s="2" t="n">
-        <v>47.74</v>
-      </c>
-    </row>
-    <row r="255" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A255" s="4" t="n">
-        <v>43494.0416666667</v>
-      </c>
-      <c r="B255" s="2" t="n">
-        <v>61.45</v>
-      </c>
-      <c r="C255" s="2" t="n">
-        <v>46.74</v>
       </c>
     </row>
   </sheetData>
@@ -14681,13 +14501,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L28" activeCellId="1" sqref="A:A L28"/>
+      <selection pane="topLeft" activeCell="L28" activeCellId="0" sqref="L28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="9.14"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -14707,14 +14524,11 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M28" activeCellId="1" sqref="A:A M28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M28" activeCellId="0" sqref="M28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="9.14"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>